<commit_message>
Chanmge the format of the driver worksheet name
Now must be the same as the pump sheet, with the word pump replaced by the word driver
</commit_message>
<xml_diff>
--- a/DHLLDV_viewer/static/pipelines/Example_input.xlsx
+++ b/DHLLDV_viewer/static/pipelines/Example_input.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcrii\PycharmProjects\DHLLDV\DHLLDV_viewer\static\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C60ABCF-EF57-40F7-A6A5-8CEDC0232C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378CDEE4-161D-49E2-99C2-30849B2EDC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipeline" sheetId="11" r:id="rId1"/>
     <sheet name="UWPump" sheetId="14" r:id="rId2"/>
     <sheet name="MainPump" sheetId="12" r:id="rId3"/>
-    <sheet name="MainPump Driver" sheetId="13" r:id="rId4"/>
+    <sheet name="MainDriver" sheetId="13" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="avail_power" localSheetId="2">MainPump!$D$10</definedName>
@@ -25,14 +25,14 @@
     <definedName name="CFS_to_GPM" localSheetId="1">UWPump!$I$1</definedName>
     <definedName name="discharge" localSheetId="2">MainPump!$D$6</definedName>
     <definedName name="discharge" localSheetId="1">UWPump!$D$6</definedName>
-    <definedName name="driver_name" localSheetId="3">'MainPump Driver'!$B$1</definedName>
-    <definedName name="gear_ratio" localSheetId="3">'MainPump Driver'!$B$3</definedName>
+    <definedName name="driver_name" localSheetId="3">MainDriver!$B$1</definedName>
+    <definedName name="gear_ratio" localSheetId="3">MainDriver!$B$3</definedName>
     <definedName name="impeller" localSheetId="2">MainPump!$D$4</definedName>
     <definedName name="impeller" localSheetId="1">UWPump!$D$4</definedName>
     <definedName name="limited" localSheetId="2">MainPump!$D$9</definedName>
     <definedName name="limited" localSheetId="1">UWPump!$D$9</definedName>
     <definedName name="pipeline_name" localSheetId="0">Pipeline!$B$1</definedName>
-    <definedName name="power_curve" localSheetId="3">'MainPump Driver'!$D$5:$E$14</definedName>
+    <definedName name="power_curve" localSheetId="3">MainDriver!$D$5:$E$14</definedName>
     <definedName name="pump_curve" localSheetId="2">MainPump!$H$13:$J$29</definedName>
     <definedName name="pump_curve" localSheetId="1">UWPump!$H$13:$J$29</definedName>
     <definedName name="pump_name" localSheetId="2">MainPump!$B$2</definedName>
@@ -2402,7 +2402,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'MainPump Driver'!$B$5</c:f>
+              <c:f>MainDriver!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2437,7 +2437,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'MainPump Driver'!$A$6:$A$14</c:f>
+              <c:f>MainDriver!$A$6:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2473,7 +2473,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'MainPump Driver'!$B$6:$B$14</c:f>
+              <c:f>MainDriver!$B$6:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="9"/>
@@ -5889,8 +5889,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5939,8 +5939,8 @@
         <v>10</v>
       </c>
       <c r="J4" t="str">
-        <f>'MainPump Driver'!driver_name</f>
-        <v>EMD 710-20-E23</v>
+        <f>MainPump!pump_name</f>
+        <v>0.864x0.864x2.134m Pump at 315 RPM</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
@@ -6040,7 +6040,7 @@
         <v>77</v>
       </c>
       <c r="B10">
-        <f>'MainPump Driver'!B14</f>
+        <f>MainDriver!B14</f>
         <v>5000</v>
       </c>
       <c r="C10" t="s">
@@ -7080,7 +7080,7 @@
         <v>77</v>
       </c>
       <c r="B10">
-        <f>'MainPump Driver'!B14</f>
+        <f>MainDriver!B14</f>
         <v>5000</v>
       </c>
       <c r="C10" t="s">
@@ -7973,7 +7973,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change range names top match Pump object parameters
</commit_message>
<xml_diff>
--- a/DHLLDV_viewer/static/pipelines/Example_input.xlsx
+++ b/DHLLDV_viewer/static/pipelines/Example_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcrii\PycharmProjects\DHLLDV\DHLLDV_viewer\static\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378CDEE4-161D-49E2-99C2-30849B2EDC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934B4C02-F6F0-4E14-A58E-FE443B548A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipeline" sheetId="11" r:id="rId1"/>
@@ -19,28 +19,29 @@
     <sheet name="MainDriver" sheetId="13" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="avail_power" localSheetId="2">MainPump!$D$10</definedName>
-    <definedName name="avail_power" localSheetId="1">UWPump!$D$10</definedName>
+    <definedName name="avail_power" localSheetId="2">MainPump!$D$11</definedName>
+    <definedName name="avail_power" localSheetId="1">UWPump!$D$11</definedName>
     <definedName name="CFS_to_GPM" localSheetId="2">MainPump!$I$1</definedName>
     <definedName name="CFS_to_GPM" localSheetId="1">UWPump!$I$1</definedName>
-    <definedName name="discharge" localSheetId="2">MainPump!$D$6</definedName>
-    <definedName name="discharge" localSheetId="1">UWPump!$D$6</definedName>
-    <definedName name="driver_name" localSheetId="3">MainDriver!$B$1</definedName>
-    <definedName name="gear_ratio" localSheetId="3">MainDriver!$B$3</definedName>
-    <definedName name="impeller" localSheetId="2">MainPump!$D$4</definedName>
-    <definedName name="impeller" localSheetId="1">UWPump!$D$4</definedName>
+    <definedName name="design_impeller" localSheetId="2">MainPump!$D$4</definedName>
+    <definedName name="design_impeller" localSheetId="1">UWPump!$D$4</definedName>
+    <definedName name="design_speed" localSheetId="2">MainPump!$D$7</definedName>
+    <definedName name="design_speed" localSheetId="1">UWPump!$D$7</definedName>
+    <definedName name="disch_dia" localSheetId="2">MainPump!$D$6</definedName>
+    <definedName name="disch_dia" localSheetId="1">UWPump!$D$6</definedName>
+    <definedName name="gear_ratio" localSheetId="2">MainPump!$D$10</definedName>
+    <definedName name="gear_ratio" localSheetId="1">UWPump!$D$10</definedName>
     <definedName name="limited" localSheetId="2">MainPump!$D$9</definedName>
     <definedName name="limited" localSheetId="1">UWPump!$D$9</definedName>
-    <definedName name="pipeline_name" localSheetId="0">Pipeline!$B$1</definedName>
-    <definedName name="power_curve" localSheetId="3">MainDriver!$D$5:$E$14</definedName>
-    <definedName name="pump_curve" localSheetId="2">MainPump!$H$13:$J$29</definedName>
-    <definedName name="pump_curve" localSheetId="1">UWPump!$H$13:$J$29</definedName>
-    <definedName name="pump_name" localSheetId="2">MainPump!$B$2</definedName>
-    <definedName name="pump_name" localSheetId="1">UWPump!$B$2</definedName>
-    <definedName name="speed" localSheetId="2">MainPump!$D$7</definedName>
-    <definedName name="speed" localSheetId="1">UWPump!$D$7</definedName>
-    <definedName name="suction" localSheetId="2">MainPump!$D$5</definedName>
-    <definedName name="suction" localSheetId="1">UWPump!$D$5</definedName>
+    <definedName name="name" localSheetId="3">MainDriver!$B$1</definedName>
+    <definedName name="name" localSheetId="2">MainPump!$B$2</definedName>
+    <definedName name="name" localSheetId="0">Pipeline!$B$1</definedName>
+    <definedName name="name" localSheetId="1">UWPump!$B$2</definedName>
+    <definedName name="power_curve" localSheetId="3">MainDriver!$D$3:$E$12</definedName>
+    <definedName name="pump_curve" localSheetId="2">MainPump!$H$14:$J$30</definedName>
+    <definedName name="pump_curve" localSheetId="1">UWPump!$H$14:$J$30</definedName>
+    <definedName name="suction_dia" localSheetId="2">MainPump!$D$5</definedName>
+    <definedName name="suction_dia" localSheetId="1">UWPump!$D$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
   <si>
     <t>Eff</t>
   </si>
@@ -307,6 +308,9 @@
   </si>
   <si>
     <t>Speed</t>
+  </si>
+  <si>
+    <t>torque</t>
   </si>
 </sst>
 </file>
@@ -445,7 +449,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -507,9 +511,7 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -518,19 +520,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -679,7 +678,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>UWPump!$B$14:$B$29</c:f>
+              <c:f>UWPump!$B$15:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
@@ -736,7 +735,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>UWPump!$C$14:$C$29</c:f>
+              <c:f>UWPump!$C$15:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -879,7 +878,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>UWPump!$B$14:$B$29</c:f>
+              <c:f>UWPump!$B$15:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
@@ -936,7 +935,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>UWPump!$D$14:$D$29</c:f>
+              <c:f>UWPump!$D$15:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1090,7 +1089,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>UWPump!$B$14:$B$29</c:f>
+              <c:f>UWPump!$B$15:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1147,7 +1146,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>UWPump!$E$14:$E$29</c:f>
+              <c:f>UWPump!$E$15:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1567,7 +1566,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>MainPump!$B$14:$B$29</c:f>
+              <c:f>MainPump!$B$15:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1624,7 +1623,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MainPump!$C$14:$C$29</c:f>
+              <c:f>MainPump!$C$15:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1767,7 +1766,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>MainPump!$B$14:$B$29</c:f>
+              <c:f>MainPump!$B$15:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1824,7 +1823,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MainPump!$D$14:$D$29</c:f>
+              <c:f>MainPump!$D$15:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1978,7 +1977,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>MainPump!$B$14:$B$29</c:f>
+              <c:f>MainPump!$B$15:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2035,7 +2034,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MainPump!$E$14:$E$29</c:f>
+              <c:f>MainPump!$E$15:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2402,7 +2401,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>MainDriver!$B$5</c:f>
+              <c:f>MainDriver!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2437,7 +2436,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>MainDriver!$A$6:$A$14</c:f>
+              <c:f>MainDriver!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2473,7 +2472,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MainDriver!$B$6:$B$14</c:f>
+              <c:f>MainDriver!$B$4:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="9"/>
@@ -4375,13 +4374,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>128587</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>568325</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4418,13 +4417,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>128587</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>568325</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4461,13 +4460,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>93662</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>179387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>274637</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>26987</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4811,7 +4810,7 @@
       <c r="A1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5887,10 +5886,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE75FAE-D548-4445-83E4-D7197FA8A6DC}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:AB46"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5917,7 +5916,7 @@
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="44" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5931,16 +5930,12 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="47">
         <f>B4*0.3048/12</f>
         <v>1.524</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
-      </c>
-      <c r="J4" t="str">
-        <f>MainPump!pump_name</f>
-        <v>0.864x0.864x2.134m Pump at 315 RPM</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
@@ -5953,7 +5948,7 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="53">
+      <c r="D5" s="47">
         <f>B5*0.3048/12</f>
         <v>0.86360000000000003</v>
       </c>
@@ -5971,7 +5966,7 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="53">
+      <c r="D6" s="47">
         <f>B6*0.3048/12</f>
         <v>0.86360000000000003</v>
       </c>
@@ -5999,7 +5994,7 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="47">
         <f>B7/60</f>
         <v>5</v>
       </c>
@@ -6022,8 +6017,8 @@
       <c r="A9" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="54" t="s">
-        <v>74</v>
+      <c r="D9" s="48" t="s">
+        <v>82</v>
       </c>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -6037,47 +6032,28 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10">
-        <f>MainDriver!B14</f>
-        <v>5000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="49">
-        <f>B10*0.7457</f>
-        <v>3728.5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="D10" s="51">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="B11">
-        <v>32.14</v>
+        <v>2000</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>9.81</v>
+        <v>4</v>
+      </c>
+      <c r="D11" s="45">
+        <f>B11*0.7457</f>
+        <v>1491.4</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
@@ -6089,837 +6065,863 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>32.14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>9.81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>15</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="49" t="s">
+      <c r="H14" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="49" t="s">
+      <c r="I14" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="J13" s="49" t="s">
+      <c r="J14" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="K13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
-        <v>0</v>
-      </c>
-      <c r="B14" s="45">
-        <f t="shared" ref="B14:B29" si="0">A14*$H$6*CFS_to_GPM</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="36">
-        <v>112.07804413656908</v>
-      </c>
-      <c r="D14" s="47">
-        <f t="shared" ref="D14:D29" si="1">100*C14*B14/(3960*E14)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="37">
-        <v>200</v>
-      </c>
-      <c r="F14" s="43"/>
-      <c r="G14">
-        <f t="shared" ref="G14:G29" si="2">A14*0.3048</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="49">
-        <f t="shared" ref="H14:H29" si="3">B14*0.0000630902</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="49">
-        <f t="shared" ref="I14:I29" si="4">C14*0.3048</f>
-        <v>34.161387852826259</v>
-      </c>
-      <c r="J14" s="50">
-        <f t="shared" ref="J14:J17" si="5">+E14*0.7457</f>
-        <v>149.14000000000001</v>
-      </c>
-      <c r="K14" s="2">
-        <f t="shared" ref="K14:K17" si="6">$D$11*H14*I14/J14</f>
+      <c r="K14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
-        <v>2</v>
-      </c>
-      <c r="B15" s="45">
-        <f t="shared" si="0"/>
-        <v>5659.760636050989</v>
+        <v>0</v>
+      </c>
+      <c r="B15" s="43">
+        <f>A15*$H$6*CFS_to_GPM</f>
+        <v>0</v>
       </c>
       <c r="C15" s="36">
-        <v>111.90921143946368</v>
-      </c>
-      <c r="D15" s="47">
-        <f t="shared" si="1"/>
-        <v>44.993114593352345</v>
+        <v>112.07804413656908</v>
+      </c>
+      <c r="D15" s="13">
+        <f t="shared" ref="D15:D30" si="0">100*C15*B15/(3960*E15)</f>
+        <v>0</v>
       </c>
       <c r="E15" s="37">
-        <v>355.48612643742598</v>
-      </c>
-      <c r="F15" s="43"/>
+        <v>200</v>
+      </c>
+      <c r="F15" s="41"/>
       <c r="G15">
-        <f t="shared" si="2"/>
-        <v>0.60960000000000003</v>
-      </c>
-      <c r="H15" s="49">
-        <f t="shared" si="3"/>
-        <v>0.3570754304805841</v>
-      </c>
-      <c r="I15" s="49">
-        <f t="shared" si="4"/>
-        <v>34.109927646748531</v>
-      </c>
-      <c r="J15" s="50">
-        <f t="shared" si="5"/>
-        <v>265.08600448438858</v>
+        <f t="shared" ref="G15:G30" si="1">A15*0.3048</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="45">
+        <f t="shared" ref="H15:H30" si="2">B15*0.0000630902</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="45">
+        <f t="shared" ref="I15:I30" si="3">C15*0.3048</f>
+        <v>34.161387852826259</v>
+      </c>
+      <c r="J15" s="46">
+        <f t="shared" ref="J15:J18" si="4">+E15*0.7457</f>
+        <v>149.14000000000001</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="6"/>
-        <v>0.45073675603887309</v>
+        <f t="shared" ref="K15:K18" si="5">$D$12*H15*I15/J15</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
+        <v>2</v>
+      </c>
+      <c r="B16" s="43">
+        <f>A16*$H$6*CFS_to_GPM</f>
+        <v>5659.760636050989</v>
+      </c>
+      <c r="C16" s="36">
+        <v>111.90921143946368</v>
+      </c>
+      <c r="D16" s="13">
+        <f t="shared" si="0"/>
+        <v>44.993114593352345</v>
+      </c>
+      <c r="E16" s="37">
+        <v>355.48612643742598</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>0.60960000000000003</v>
+      </c>
+      <c r="H16" s="45">
+        <f t="shared" si="2"/>
+        <v>0.3570754304805841</v>
+      </c>
+      <c r="I16" s="45">
+        <f t="shared" si="3"/>
+        <v>34.109927646748531</v>
+      </c>
+      <c r="J16" s="46">
+        <f t="shared" si="4"/>
+        <v>265.08600448438858</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="5"/>
+        <v>0.45073675603887309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="45">
+      <c r="B17" s="43">
+        <f>A17*$H$6*CFS_to_GPM</f>
+        <v>11319.521272101978</v>
+      </c>
+      <c r="C17" s="36">
+        <v>111.44640296562086</v>
+      </c>
+      <c r="D17" s="13">
         <f t="shared" si="0"/>
-        <v>11319.521272101978</v>
-      </c>
-      <c r="C16" s="36">
-        <v>111.44640296562086</v>
-      </c>
-      <c r="D16" s="47">
+        <v>58.366433328998852</v>
+      </c>
+      <c r="E17" s="37">
+        <v>545.80281933281822</v>
+      </c>
+      <c r="F17" s="41"/>
+      <c r="G17">
         <f t="shared" si="1"/>
-        <v>58.366433328998852</v>
-      </c>
-      <c r="E16" s="37">
-        <v>545.80281933281822</v>
-      </c>
-      <c r="F16" s="43"/>
-      <c r="G16">
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="H17" s="45">
         <f t="shared" si="2"/>
-        <v>1.2192000000000001</v>
-      </c>
-      <c r="H16" s="49">
+        <v>0.7141508609611682</v>
+      </c>
+      <c r="I17" s="45">
         <f t="shared" si="3"/>
-        <v>0.7141508609611682</v>
-      </c>
-      <c r="I16" s="49">
+        <v>33.968863623921237</v>
+      </c>
+      <c r="J17" s="46">
         <f t="shared" si="4"/>
-        <v>33.968863623921237</v>
-      </c>
-      <c r="J16" s="50">
+        <v>407.00516237648259</v>
+      </c>
+      <c r="K17" s="2">
         <f t="shared" si="5"/>
-        <v>407.00516237648259</v>
-      </c>
-      <c r="K16" s="2">
-        <f t="shared" si="6"/>
         <v>0.58470939516063303</v>
       </c>
     </row>
-    <row r="17" spans="1:25" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="39">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
         <v>6</v>
       </c>
-      <c r="B17" s="45">
+      <c r="B18" s="43">
+        <f>A18*$H$6*CFS_to_GPM</f>
+        <v>16979.281908152967</v>
+      </c>
+      <c r="C18" s="36">
+        <v>110.65381637119108</v>
+      </c>
+      <c r="D18" s="13">
         <f t="shared" si="0"/>
-        <v>16979.281908152967</v>
-      </c>
-      <c r="C17" s="46">
-        <v>110.65381637119108</v>
-      </c>
-      <c r="D17" s="47">
+        <v>66.25243467148313</v>
+      </c>
+      <c r="E18" s="39">
+        <v>716.12475648939767</v>
+      </c>
+      <c r="F18" s="42"/>
+      <c r="G18">
         <f t="shared" si="1"/>
-        <v>66.25243467148313</v>
-      </c>
-      <c r="E17" s="40">
-        <v>716.12475648939767</v>
-      </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="41">
+        <v>1.8288000000000002</v>
+      </c>
+      <c r="H18" s="45">
         <f t="shared" si="2"/>
-        <v>1.8288000000000002</v>
-      </c>
-      <c r="H17" s="51">
+        <v>1.0712262914417523</v>
+      </c>
+      <c r="I18" s="45">
         <f t="shared" si="3"/>
-        <v>1.0712262914417523</v>
-      </c>
-      <c r="I17" s="51">
+        <v>33.727283229939047</v>
+      </c>
+      <c r="J18" s="46">
         <f t="shared" si="4"/>
-        <v>33.727283229939047</v>
-      </c>
-      <c r="J17" s="52">
+        <v>534.01423091414381</v>
+      </c>
+      <c r="K18" s="40">
         <f t="shared" si="5"/>
-        <v>534.01423091414381</v>
-      </c>
-      <c r="K17" s="42">
-        <f t="shared" si="6"/>
         <v>0.66371060890978628</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
-        <v>8</v>
-      </c>
-      <c r="B18" s="45">
-        <f t="shared" si="0"/>
-        <v>22639.042544203956</v>
-      </c>
-      <c r="C18" s="36">
-        <v>109.51051504641677</v>
-      </c>
-      <c r="D18" s="47">
-        <f t="shared" si="1"/>
-        <v>71.418090136807777</v>
-      </c>
-      <c r="E18" s="38">
-        <v>876.61815166325812</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="2"/>
-        <v>2.4384000000000001</v>
-      </c>
-      <c r="H18" s="49">
-        <f t="shared" si="3"/>
-        <v>1.4283017219223364</v>
-      </c>
-      <c r="I18" s="49">
-        <f t="shared" si="4"/>
-        <v>33.378804986147834</v>
-      </c>
-      <c r="J18" s="50">
-        <f>+E18*0.7457</f>
-        <v>653.69415569529156</v>
-      </c>
-      <c r="K18" s="2">
-        <f>$D$11*H18*I18/J18</f>
-        <v>0.71545965558722857</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
-        <v>10</v>
-      </c>
-      <c r="B19" s="45">
+        <v>8</v>
+      </c>
+      <c r="B19" s="43">
+        <f>A19*$H$6*CFS_to_GPM</f>
+        <v>22639.042544203956</v>
+      </c>
+      <c r="C19" s="36">
+        <v>109.51051504641677</v>
+      </c>
+      <c r="D19" s="13">
         <f t="shared" si="0"/>
-        <v>28298.803180254945</v>
-      </c>
-      <c r="C19" s="36">
-        <v>108.01102837157788</v>
-      </c>
-      <c r="D19" s="47">
+        <v>71.418090136807777</v>
+      </c>
+      <c r="E19" s="38">
+        <v>876.61815166325812</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="1"/>
-        <v>74.878695252862229</v>
-      </c>
-      <c r="E19" s="38">
-        <v>1030.8197134146665</v>
-      </c>
-      <c r="G19">
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="H19" s="45">
         <f t="shared" si="2"/>
-        <v>3.048</v>
-      </c>
-      <c r="H19" s="49">
+        <v>1.4283017219223364</v>
+      </c>
+      <c r="I19" s="45">
         <f t="shared" si="3"/>
-        <v>1.7853771524029203</v>
-      </c>
-      <c r="I19" s="49">
-        <f t="shared" si="4"/>
-        <v>32.921761447656941</v>
-      </c>
-      <c r="J19" s="49">
-        <f t="shared" ref="J19:J29" si="7">+E19*0.7457</f>
-        <v>768.68226029331686</v>
+        <v>33.378804986147834</v>
+      </c>
+      <c r="J19" s="46">
+        <f>+E19*0.7457</f>
+        <v>653.69415569529156</v>
       </c>
       <c r="K19" s="2">
-        <f>$D$11*H19*I19/J19</f>
-        <v>0.75012766952757404</v>
+        <f t="shared" ref="K19:K27" si="6">$D$12*H19*I19/J19</f>
+        <v>0.71545965558722857</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
+        <v>10</v>
+      </c>
+      <c r="B20" s="43">
+        <f>A20*$H$6*CFS_to_GPM</f>
+        <v>28298.803180254945</v>
+      </c>
+      <c r="C20" s="36">
+        <v>108.01102837157788</v>
+      </c>
+      <c r="D20" s="13">
+        <f t="shared" si="0"/>
+        <v>74.878695252862229</v>
+      </c>
+      <c r="E20" s="38">
+        <v>1030.8197134146665</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>3.048</v>
+      </c>
+      <c r="H20" s="45">
+        <f t="shared" si="2"/>
+        <v>1.7853771524029203</v>
+      </c>
+      <c r="I20" s="45">
+        <f t="shared" si="3"/>
+        <v>32.921761447656941</v>
+      </c>
+      <c r="J20" s="45">
+        <f t="shared" ref="J20:J30" si="7">+E20*0.7457</f>
+        <v>768.68226029331686</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="6"/>
+        <v>0.75012766952757404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
         <v>12</v>
       </c>
-      <c r="B20" s="45">
+      <c r="B21" s="43">
+        <f>A21*$H$6*CFS_to_GPM</f>
+        <v>33958.563816305934</v>
+      </c>
+      <c r="C21" s="36">
+        <v>106.16514088523554</v>
+      </c>
+      <c r="D21" s="13">
         <f t="shared" si="0"/>
-        <v>33958.563816305934</v>
-      </c>
-      <c r="C20" s="36">
-        <v>106.16514088523554</v>
-      </c>
-      <c r="D20" s="47">
+        <v>77.109628095859165</v>
+      </c>
+      <c r="E21" s="38">
+        <v>1180.6670976329533</v>
+      </c>
+      <c r="G21">
         <f t="shared" si="1"/>
-        <v>77.109628095859165</v>
-      </c>
-      <c r="E20" s="38">
-        <v>1180.6670976329533</v>
-      </c>
-      <c r="G20">
+        <v>3.6576000000000004</v>
+      </c>
+      <c r="H21" s="45">
         <f t="shared" si="2"/>
-        <v>3.6576000000000004</v>
-      </c>
-      <c r="H20" s="49">
+        <v>2.1424525828835046</v>
+      </c>
+      <c r="I21" s="45">
         <f t="shared" si="3"/>
-        <v>2.1424525828835046</v>
-      </c>
-      <c r="I20" s="49">
-        <f t="shared" si="4"/>
         <v>32.359134941819796</v>
       </c>
-      <c r="J20" s="49">
+      <c r="J21" s="45">
         <f t="shared" si="7"/>
         <v>880.42345470489329</v>
       </c>
-      <c r="K20" s="2">
-        <f>$D$11*H20*I20/J20</f>
+      <c r="K21" s="2">
+        <f t="shared" si="6"/>
         <v>0.77247694322603466</v>
       </c>
-      <c r="Y20">
+      <c r="Y21">
         <f>0.001797851/(0.00000001908315*2)</f>
         <v>47105.718919570405</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
         <v>14</v>
       </c>
-      <c r="B21" s="45">
+      <c r="B22" s="43">
+        <f>A22*$H$6*CFS_to_GPM</f>
+        <v>39618.324452356923</v>
+      </c>
+      <c r="C22" s="36">
+        <v>103.99682513667045</v>
+      </c>
+      <c r="D22" s="13">
         <f t="shared" si="0"/>
-        <v>39618.324452356923</v>
-      </c>
-      <c r="C21" s="36">
-        <v>103.99682513667045</v>
-      </c>
-      <c r="D21" s="47">
+        <v>78.355607844983155</v>
+      </c>
+      <c r="E22" s="38">
+        <v>1327.855801945281</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="1"/>
-        <v>78.355607844983155</v>
-      </c>
-      <c r="E21" s="38">
-        <v>1327.855801945281</v>
-      </c>
-      <c r="G21">
+        <v>4.2671999999999999</v>
+      </c>
+      <c r="H22" s="45">
         <f t="shared" si="2"/>
-        <v>4.2671999999999999</v>
-      </c>
-      <c r="H21" s="49">
+        <v>2.4995280133640887</v>
+      </c>
+      <c r="I22" s="45">
         <f t="shared" si="3"/>
-        <v>2.4995280133640887</v>
-      </c>
-      <c r="I21" s="49">
-        <f t="shared" si="4"/>
         <v>31.698232301657157</v>
       </c>
-      <c r="J21" s="49">
+      <c r="J22" s="45">
         <f t="shared" si="7"/>
         <v>990.18207151059607</v>
       </c>
-      <c r="K21" s="2">
-        <f>$D$11*H21*I21/J21</f>
+      <c r="K22" s="2">
+        <f t="shared" si="6"/>
         <v>0.78495905021698409</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A22" s="6">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
         <v>16</v>
       </c>
-      <c r="B22" s="45">
+      <c r="B23" s="43">
+        <f>A23*$H$6*CFS_to_GPM</f>
+        <v>45278.085088407912</v>
+      </c>
+      <c r="C23" s="36">
+        <v>101.54239039924866</v>
+      </c>
+      <c r="D23" s="13">
         <f t="shared" si="0"/>
-        <v>45278.085088407912</v>
-      </c>
-      <c r="C22" s="36">
-        <v>101.54239039924866</v>
-      </c>
-      <c r="D22" s="47">
+        <v>78.745760545303426</v>
+      </c>
+      <c r="E23" s="38">
+        <v>1474.3923415459931</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="1"/>
-        <v>78.745760545303426</v>
-      </c>
-      <c r="E22" s="38">
-        <v>1474.3923415459931</v>
-      </c>
-      <c r="G22">
+        <v>4.8768000000000002</v>
+      </c>
+      <c r="H23" s="45">
         <f t="shared" si="2"/>
-        <v>4.8768000000000002</v>
-      </c>
-      <c r="H22" s="49">
+        <v>2.8566034438446728</v>
+      </c>
+      <c r="I23" s="45">
         <f t="shared" si="3"/>
-        <v>2.8566034438446728</v>
-      </c>
-      <c r="I22" s="49">
-        <f t="shared" si="4"/>
         <v>30.950120593690993</v>
       </c>
-      <c r="J22" s="49">
+      <c r="J23" s="45">
         <f t="shared" si="7"/>
         <v>1099.454369090847</v>
       </c>
-      <c r="K22" s="2">
-        <f>$D$11*H22*I22/J22</f>
+      <c r="K23" s="2">
+        <f t="shared" si="6"/>
         <v>0.78886756297702643</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
         <v>18</v>
       </c>
-      <c r="B23" s="45">
+      <c r="B24" s="43">
+        <f>A24*$H$6*CFS_to_GPM</f>
+        <v>50937.845724458901</v>
+      </c>
+      <c r="C24" s="36">
+        <v>98.84802155820627</v>
+      </c>
+      <c r="D24" s="13">
         <f t="shared" si="0"/>
-        <v>50937.845724458901</v>
-      </c>
-      <c r="C23" s="36">
-        <v>98.84802155820627</v>
-      </c>
-      <c r="D23" s="47">
+        <v>78.347575156743346</v>
+      </c>
+      <c r="E24" s="38">
+        <v>1622.8852365054029</v>
+      </c>
+      <c r="G24">
         <f t="shared" si="1"/>
-        <v>78.347575156743346</v>
-      </c>
-      <c r="E23" s="38">
-        <v>1622.8852365054029</v>
-      </c>
-      <c r="G23">
+        <v>5.4864000000000006</v>
+      </c>
+      <c r="H24" s="45">
         <f t="shared" si="2"/>
-        <v>5.4864000000000006</v>
-      </c>
-      <c r="H23" s="49">
+        <v>3.2136788743252565</v>
+      </c>
+      <c r="I24" s="45">
         <f t="shared" si="3"/>
-        <v>3.2136788743252565</v>
-      </c>
-      <c r="I23" s="49">
-        <f t="shared" si="4"/>
         <v>30.128876970941274</v>
       </c>
-      <c r="J23" s="49">
+      <c r="J24" s="45">
         <f t="shared" si="7"/>
         <v>1210.1855208620789</v>
       </c>
-      <c r="K23" s="2">
-        <f>$D$11*H23*I23/J23</f>
+      <c r="K24" s="2">
+        <f t="shared" si="6"/>
         <v>0.78487857950780526</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A25" s="6">
         <v>20</v>
       </c>
-      <c r="B24" s="45">
+      <c r="B25" s="43">
+        <f>A25*$H$6*CFS_to_GPM</f>
+        <v>56597.60636050989</v>
+      </c>
+      <c r="C25" s="36">
+        <v>95.966952520913182</v>
+      </c>
+      <c r="D25" s="13">
         <f t="shared" si="0"/>
-        <v>56597.60636050989</v>
-      </c>
-      <c r="C24" s="36">
-        <v>95.966952520913182</v>
-      </c>
-      <c r="D24" s="47">
+        <v>77.197318440056904</v>
+      </c>
+      <c r="E25" s="38">
+        <v>1776.7338126596146</v>
+      </c>
+      <c r="G25">
         <f t="shared" si="1"/>
-        <v>77.197318440056904</v>
-      </c>
-      <c r="E24" s="38">
-        <v>1776.7338126596146</v>
-      </c>
-      <c r="G24">
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="H25" s="45">
         <f t="shared" si="2"/>
-        <v>6.0960000000000001</v>
-      </c>
-      <c r="H24" s="49">
+        <v>3.5707543048058406</v>
+      </c>
+      <c r="I25" s="45">
         <f t="shared" si="3"/>
-        <v>3.5707543048058406</v>
-      </c>
-      <c r="I24" s="49">
-        <f t="shared" si="4"/>
         <v>29.25072712837434</v>
       </c>
-      <c r="J24" s="49">
+      <c r="J25" s="45">
         <f t="shared" si="7"/>
         <v>1324.9104041002747</v>
       </c>
-      <c r="K24" s="2">
-        <f>$D$11*H24*I24/J24</f>
+      <c r="K25" s="2">
+        <f t="shared" si="6"/>
         <v>0.77335541677997377</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A26" s="6">
         <v>22</v>
       </c>
-      <c r="B25" s="45">
+      <c r="B26" s="43">
+        <f>A26*$H$6*CFS_to_GPM</f>
+        <v>62257.366996560879</v>
+      </c>
+      <c r="C26" s="36">
+        <v>92.956547008200985</v>
+      </c>
+      <c r="D26" s="13">
         <f t="shared" si="0"/>
-        <v>62257.366996560879</v>
-      </c>
-      <c r="C25" s="36">
-        <v>92.956547008200985</v>
-      </c>
-      <c r="D25" s="47">
+        <v>75.32013568023136</v>
+      </c>
+      <c r="E26" s="38">
+        <v>1940.280204065019</v>
+      </c>
+      <c r="G26">
         <f t="shared" si="1"/>
-        <v>75.32013568023136</v>
-      </c>
-      <c r="E25" s="38">
-        <v>1940.280204065019</v>
-      </c>
-      <c r="G25">
+        <v>6.7056000000000004</v>
+      </c>
+      <c r="H26" s="45">
         <f t="shared" si="2"/>
-        <v>6.7056000000000004</v>
-      </c>
-      <c r="H25" s="49">
+        <v>3.9278297352864247</v>
+      </c>
+      <c r="I26" s="45">
         <f t="shared" si="3"/>
-        <v>3.9278297352864247</v>
-      </c>
-      <c r="I25" s="49">
-        <f t="shared" si="4"/>
         <v>28.333155528099663</v>
       </c>
-      <c r="J25" s="49">
+      <c r="J26" s="45">
         <f t="shared" si="7"/>
         <v>1446.8669481712848</v>
       </c>
-      <c r="K25" s="2">
-        <f>$D$11*H25*I25/J25</f>
+      <c r="K26" s="2">
+        <f t="shared" si="6"/>
         <v>0.75454997787442024</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A27" s="6">
         <v>24</v>
       </c>
-      <c r="B26" s="45">
+      <c r="B27" s="43">
+        <f>A27*$H$6*CFS_to_GPM</f>
+        <v>67917.127632611868</v>
+      </c>
+      <c r="C27" s="36">
+        <v>89.875546479220858</v>
+      </c>
+      <c r="D27" s="13">
         <f t="shared" si="0"/>
-        <v>67917.127632611868</v>
-      </c>
-      <c r="C26" s="36">
-        <v>89.875546479220858</v>
-      </c>
-      <c r="D26" s="47">
+        <v>72.745048933891951</v>
+      </c>
+      <c r="E27" s="38">
+        <v>2118.9574121870969</v>
+      </c>
+      <c r="G27">
         <f t="shared" si="1"/>
-        <v>72.745048933891951</v>
-      </c>
-      <c r="E26" s="38">
-        <v>2118.9574121870969</v>
-      </c>
-      <c r="G26">
+        <v>7.3152000000000008</v>
+      </c>
+      <c r="H27" s="45">
         <f t="shared" si="2"/>
-        <v>7.3152000000000008</v>
-      </c>
-      <c r="H26" s="49">
+        <v>4.2849051657670092</v>
+      </c>
+      <c r="I27" s="45">
         <f t="shared" si="3"/>
-        <v>4.2849051657670092</v>
-      </c>
-      <c r="I26" s="49">
-        <f t="shared" si="4"/>
         <v>27.39406656686652</v>
       </c>
-      <c r="J26" s="49">
+      <c r="J27" s="45">
         <f t="shared" si="7"/>
         <v>1580.1065422679183</v>
       </c>
-      <c r="K26" s="2">
-        <f>$D$11*H26*I26/J26</f>
+      <c r="K27" s="2">
+        <f t="shared" si="6"/>
         <v>0.72875300300273138</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A28" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="45">
+      <c r="B28" s="43">
+        <f>A28*$H$6*CFS_to_GPM</f>
+        <v>73576.888268662864</v>
+      </c>
+      <c r="C28" s="36">
+        <v>86.781698520794137</v>
+      </c>
+      <c r="D28" s="13">
         <f t="shared" si="0"/>
-        <v>73576.888268662864</v>
-      </c>
-      <c r="C27" s="36">
-        <v>86.781698520794137</v>
-      </c>
-      <c r="D27" s="47">
+        <v>69.516853126649153</v>
+      </c>
+      <c r="E28" s="38">
+        <v>2319.446034112932</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="1"/>
-        <v>69.516853126649153</v>
-      </c>
-      <c r="E27" s="38">
-        <v>2319.446034112932</v>
-      </c>
-      <c r="G27">
+        <v>7.9248000000000003</v>
+      </c>
+      <c r="H28" s="45">
         <f t="shared" si="2"/>
-        <v>7.9248000000000003</v>
-      </c>
-      <c r="H27" s="49">
+        <v>4.6419805962475937</v>
+      </c>
+      <c r="I28" s="45">
         <f t="shared" si="3"/>
-        <v>4.6419805962475937</v>
-      </c>
-      <c r="I27" s="49">
-        <f t="shared" si="4"/>
         <v>26.451061709138056</v>
       </c>
-      <c r="J27" s="49">
+      <c r="J28" s="45">
         <f t="shared" si="7"/>
         <v>1729.6109076380135</v>
       </c>
-      <c r="K27" s="2">
-        <f t="shared" ref="K27" si="8">$D$11*H27*I27/J27</f>
+      <c r="K28" s="2">
+        <f t="shared" ref="K28" si="8">$D$12*H28*I28/J28</f>
         <v>0.69641324348250722</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B28" s="45">
+      <c r="B29" s="43">
+        <f>A29*$H$6*CFS_to_GPM</f>
+        <v>79236.648904713846</v>
+      </c>
+      <c r="C29" s="36">
+        <v>83.729912882852531</v>
+      </c>
+      <c r="D29" s="13">
         <f t="shared" si="0"/>
-        <v>79236.648904713846</v>
-      </c>
-      <c r="C28" s="36">
-        <v>83.729912882852531</v>
-      </c>
-      <c r="D28" s="47">
+        <v>65.705382939207482</v>
+      </c>
+      <c r="E29" s="38">
+        <v>2549.8263370917853</v>
+      </c>
+      <c r="G29">
         <f t="shared" si="1"/>
-        <v>65.705382939207482</v>
-      </c>
-      <c r="E28" s="38">
-        <v>2549.8263370917853</v>
-      </c>
-      <c r="G28">
+        <v>8.5343999999999998</v>
+      </c>
+      <c r="H29" s="45">
         <f t="shared" si="2"/>
-        <v>8.5343999999999998</v>
-      </c>
-      <c r="H28" s="49">
+        <v>4.9990560267281774</v>
+      </c>
+      <c r="I29" s="45">
         <f t="shared" si="3"/>
-        <v>4.9990560267281774</v>
-      </c>
-      <c r="I28" s="49">
-        <f t="shared" si="4"/>
         <v>25.520877446693454</v>
       </c>
-      <c r="J28" s="49">
+      <c r="J29" s="45">
         <f t="shared" si="7"/>
         <v>1901.4054995693443</v>
       </c>
-      <c r="K28" s="2">
-        <f>$D$11*H28*I28/J28</f>
+      <c r="K29" s="2">
+        <f>$D$12*H29*I29/J29</f>
         <v>0.65823029652377052</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A30" s="6">
         <v>30</v>
       </c>
-      <c r="B29" s="45">
+      <c r="B30" s="43">
+        <f>A30*$H$6*CFS_to_GPM</f>
+        <v>84896.409540764827</v>
+      </c>
+      <c r="C30" s="36">
+        <v>80.771021393068821</v>
+      </c>
+      <c r="D30" s="13">
         <f t="shared" si="0"/>
-        <v>84896.409540764827</v>
-      </c>
-      <c r="C29" s="36">
-        <v>80.771021393068821</v>
-      </c>
-      <c r="D29" s="47">
+        <v>61.41179783287653</v>
+      </c>
+      <c r="E30" s="38">
+        <v>2819.6675134712896</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="1"/>
-        <v>61.41179783287653</v>
-      </c>
-      <c r="E29" s="38">
-        <v>2819.6675134712896</v>
-      </c>
-      <c r="G29">
+        <v>9.1440000000000001</v>
+      </c>
+      <c r="H30" s="45">
         <f t="shared" si="2"/>
-        <v>9.1440000000000001</v>
-      </c>
-      <c r="H29" s="49">
+        <v>5.356131457208761</v>
+      </c>
+      <c r="I30" s="45">
         <f t="shared" si="3"/>
-        <v>5.356131457208761</v>
-      </c>
-      <c r="I29" s="49">
-        <f t="shared" si="4"/>
         <v>24.619007320607377</v>
       </c>
-      <c r="J29" s="49">
+      <c r="J30" s="45">
         <f t="shared" si="7"/>
         <v>2102.6260647955405</v>
       </c>
-      <c r="K29" s="2">
-        <f>$D$11*H29*I29/J29</f>
+      <c r="K30" s="2">
+        <f>$D$12*H30*I30/J30</f>
         <v>0.61521756801863225</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="K30" s="2"/>
-    </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="H31" t="str">
-        <f>TEXT(H14,"0.0000000")&amp;": "&amp;TEXT(I14,"0.000000")&amp;","</f>
-        <v>0.0000000: 34.161388,</v>
-      </c>
-      <c r="J31" t="str">
-        <f>TEXT(H14,"0.000000")&amp;": "&amp;TEXT(J14,"0.000000")&amp;","</f>
-        <v>0.000000: 149.140000,</v>
-      </c>
+      <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="H32" t="str">
-        <f>TEXT(H15,"0.0000000")&amp;": "&amp;TEXT(I15,"0.000000")&amp;","</f>
-        <v>0.3570754: 34.109928,</v>
+        <f t="shared" ref="H32:H47" si="9">TEXT(H15,"0.0000000")&amp;": "&amp;TEXT(I15,"0.000000")&amp;","</f>
+        <v>0.0000000: 34.161388,</v>
       </c>
       <c r="J32" t="str">
-        <f>TEXT(H15,"0.000000")&amp;": "&amp;TEXT(J15,"0.000000")&amp;","</f>
-        <v>0.357075: 265.086004,</v>
+        <f t="shared" ref="J32:J47" si="10">TEXT(H15,"0.000000")&amp;": "&amp;TEXT(J15,"0.000000")&amp;","</f>
+        <v>0.000000: 149.140000,</v>
       </c>
     </row>
     <row r="33" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H33" t="str">
-        <f>TEXT(H16,"0.0000000")&amp;": "&amp;TEXT(I16,"0.000000")&amp;","</f>
-        <v>0.7141509: 33.968864,</v>
+        <f t="shared" si="9"/>
+        <v>0.3570754: 34.109928,</v>
       </c>
       <c r="J33" t="str">
-        <f>TEXT(H16,"0.000000")&amp;": "&amp;TEXT(J16,"0.000000")&amp;","</f>
-        <v>0.714151: 407.005162,</v>
+        <f t="shared" si="10"/>
+        <v>0.357075: 265.086004,</v>
       </c>
     </row>
     <row r="34" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H34" t="str">
-        <f>TEXT(H17,"0.0000000")&amp;": "&amp;TEXT(I17,"0.000000")&amp;","</f>
-        <v>1.0712263: 33.727283,</v>
+        <f t="shared" si="9"/>
+        <v>0.7141509: 33.968864,</v>
       </c>
       <c r="J34" t="str">
-        <f>TEXT(H17,"0.000000")&amp;": "&amp;TEXT(J17,"0.000000")&amp;","</f>
-        <v>1.071226: 534.014231,</v>
+        <f t="shared" si="10"/>
+        <v>0.714151: 407.005162,</v>
       </c>
     </row>
     <row r="35" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H35" t="str">
-        <f>TEXT(H18,"0.0000000")&amp;": "&amp;TEXT(I18,"0.000000")&amp;","</f>
-        <v>1.4283017: 33.378805,</v>
+        <f t="shared" si="9"/>
+        <v>1.0712263: 33.727283,</v>
       </c>
       <c r="J35" t="str">
-        <f>TEXT(H18,"0.000000")&amp;": "&amp;TEXT(J18,"0.000000")&amp;","</f>
-        <v>1.428302: 653.694156,</v>
+        <f t="shared" si="10"/>
+        <v>1.071226: 534.014231,</v>
       </c>
     </row>
     <row r="36" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H36" t="str">
-        <f>TEXT(H19,"0.0000000")&amp;": "&amp;TEXT(I19,"0.000000")&amp;","</f>
-        <v>1.7853772: 32.921761,</v>
+        <f t="shared" si="9"/>
+        <v>1.4283017: 33.378805,</v>
       </c>
       <c r="J36" t="str">
-        <f>TEXT(H19,"0.000000")&amp;": "&amp;TEXT(J19,"0.000000")&amp;","</f>
-        <v>1.785377: 768.682260,</v>
+        <f t="shared" si="10"/>
+        <v>1.428302: 653.694156,</v>
       </c>
     </row>
     <row r="37" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H37" t="str">
-        <f>TEXT(H20,"0.0000000")&amp;": "&amp;TEXT(I20,"0.000000")&amp;","</f>
-        <v>2.1424526: 32.359135,</v>
+        <f t="shared" si="9"/>
+        <v>1.7853772: 32.921761,</v>
       </c>
       <c r="J37" t="str">
-        <f>TEXT(H20,"0.000000")&amp;": "&amp;TEXT(J20,"0.000000")&amp;","</f>
-        <v>2.142453: 880.423455,</v>
+        <f t="shared" si="10"/>
+        <v>1.785377: 768.682260,</v>
       </c>
     </row>
     <row r="38" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H38" t="str">
-        <f>TEXT(H21,"0.0000000")&amp;": "&amp;TEXT(I21,"0.000000")&amp;","</f>
-        <v>2.4995280: 31.698232,</v>
+        <f t="shared" si="9"/>
+        <v>2.1424526: 32.359135,</v>
       </c>
       <c r="J38" t="str">
-        <f>TEXT(H21,"0.000000")&amp;": "&amp;TEXT(J21,"0.000000")&amp;","</f>
-        <v>2.499528: 990.182072,</v>
+        <f t="shared" si="10"/>
+        <v>2.142453: 880.423455,</v>
       </c>
     </row>
     <row r="39" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H39" t="str">
-        <f>TEXT(H22,"0.0000000")&amp;": "&amp;TEXT(I22,"0.000000")&amp;","</f>
-        <v>2.8566034: 30.950121,</v>
+        <f t="shared" si="9"/>
+        <v>2.4995280: 31.698232,</v>
       </c>
       <c r="J39" t="str">
-        <f>TEXT(H22,"0.000000")&amp;": "&amp;TEXT(J22,"0.000000")&amp;","</f>
-        <v>2.856603: 1099.454369,</v>
+        <f t="shared" si="10"/>
+        <v>2.499528: 990.182072,</v>
       </c>
     </row>
     <row r="40" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H40" t="str">
-        <f>TEXT(H23,"0.0000000")&amp;": "&amp;TEXT(I23,"0.000000")&amp;","</f>
-        <v>3.2136789: 30.128877,</v>
+        <f t="shared" si="9"/>
+        <v>2.8566034: 30.950121,</v>
       </c>
       <c r="J40" t="str">
-        <f>TEXT(H23,"0.000000")&amp;": "&amp;TEXT(J23,"0.000000")&amp;","</f>
-        <v>3.213679: 1210.185521,</v>
+        <f t="shared" si="10"/>
+        <v>2.856603: 1099.454369,</v>
       </c>
     </row>
     <row r="41" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H41" t="str">
-        <f>TEXT(H24,"0.0000000")&amp;": "&amp;TEXT(I24,"0.000000")&amp;","</f>
-        <v>3.5707543: 29.250727,</v>
+        <f t="shared" si="9"/>
+        <v>3.2136789: 30.128877,</v>
       </c>
       <c r="J41" t="str">
-        <f>TEXT(H24,"0.000000")&amp;": "&amp;TEXT(J24,"0.000000")&amp;","</f>
-        <v>3.570754: 1324.910404,</v>
+        <f t="shared" si="10"/>
+        <v>3.213679: 1210.185521,</v>
       </c>
     </row>
     <row r="42" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H42" t="str">
-        <f>TEXT(H25,"0.0000000")&amp;": "&amp;TEXT(I25,"0.000000")&amp;","</f>
-        <v>3.9278297: 28.333156,</v>
+        <f t="shared" si="9"/>
+        <v>3.5707543: 29.250727,</v>
       </c>
       <c r="J42" t="str">
-        <f>TEXT(H25,"0.000000")&amp;": "&amp;TEXT(J25,"0.000000")&amp;","</f>
-        <v>3.927830: 1446.866948,</v>
+        <f t="shared" si="10"/>
+        <v>3.570754: 1324.910404,</v>
       </c>
     </row>
     <row r="43" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H43" t="str">
-        <f>TEXT(H26,"0.0000000")&amp;": "&amp;TEXT(I26,"0.000000")&amp;","</f>
-        <v>4.2849052: 27.394067,</v>
+        <f t="shared" si="9"/>
+        <v>3.9278297: 28.333156,</v>
       </c>
       <c r="J43" t="str">
-        <f>TEXT(H26,"0.000000")&amp;": "&amp;TEXT(J26,"0.000000")&amp;","</f>
-        <v>4.284905: 1580.106542,</v>
+        <f t="shared" si="10"/>
+        <v>3.927830: 1446.866948,</v>
       </c>
     </row>
     <row r="44" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H44" t="str">
-        <f>TEXT(H27,"0.0000000")&amp;": "&amp;TEXT(I27,"0.000000")&amp;","</f>
-        <v>4.6419806: 26.451062,</v>
+        <f t="shared" si="9"/>
+        <v>4.2849052: 27.394067,</v>
       </c>
       <c r="J44" t="str">
-        <f>TEXT(H27,"0.000000")&amp;": "&amp;TEXT(J27,"0.000000")&amp;","</f>
-        <v>4.641981: 1729.610908,</v>
+        <f t="shared" si="10"/>
+        <v>4.284905: 1580.106542,</v>
       </c>
     </row>
     <row r="45" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H45" t="str">
-        <f>TEXT(H28,"0.0000000")&amp;": "&amp;TEXT(I28,"0.000000")&amp;","</f>
-        <v>4.9990560: 25.520877,</v>
+        <f t="shared" si="9"/>
+        <v>4.6419806: 26.451062,</v>
       </c>
       <c r="J45" t="str">
-        <f>TEXT(H28,"0.000000")&amp;": "&amp;TEXT(J28,"0.000000")&amp;","</f>
-        <v>4.999056: 1901.405500,</v>
+        <f t="shared" si="10"/>
+        <v>4.641981: 1729.610908,</v>
       </c>
     </row>
     <row r="46" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H46" t="str">
-        <f>TEXT(H29,"0.0000000")&amp;": "&amp;TEXT(I29,"0.000000")&amp;","</f>
+        <f t="shared" si="9"/>
+        <v>4.9990560: 25.520877,</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="10"/>
+        <v>4.999056: 1901.405500,</v>
+      </c>
+    </row>
+    <row r="47" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H47" t="str">
+        <f t="shared" si="9"/>
         <v>5.3561315: 24.619007,</v>
       </c>
-      <c r="J46" t="str">
-        <f>TEXT(H29,"0.000000")&amp;": "&amp;TEXT(J29,"0.000000")&amp;","</f>
+      <c r="J47" t="str">
+        <f t="shared" si="10"/>
         <v>5.356131: 2102.626065,</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>$B$10/$B$11</formula>
+      <formula>$B$11/$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6931,10 +6933,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9828F5-8C39-4437-8C3A-A3686103312A}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:AB46"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6961,7 +6963,7 @@
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="44" t="s">
         <v>73</v>
       </c>
     </row>
@@ -6975,7 +6977,7 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="47">
         <f>B4*0.3048/12</f>
         <v>2.1335999999999999</v>
       </c>
@@ -6993,7 +6995,7 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="53">
+      <c r="D5" s="47">
         <f>B5*0.3048/12</f>
         <v>0.86360000000000003</v>
       </c>
@@ -7011,7 +7013,7 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="53">
+      <c r="D6" s="47">
         <f>B6*0.3048/12</f>
         <v>0.86360000000000003</v>
       </c>
@@ -7039,7 +7041,7 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="47">
         <f>B7/60</f>
         <v>5.25</v>
       </c>
@@ -7062,7 +7064,7 @@
       <c r="A9" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="48" t="s">
         <v>74</v>
       </c>
       <c r="T9" s="3"/>
@@ -7077,21 +7079,11 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10">
-        <f>MainDriver!B14</f>
-        <v>5000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="49">
-        <f>B10*0.7457</f>
-        <v>3728.5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="D10" s="45">
+        <f>MainDriver!D12/MainPump!design_speed</f>
+        <v>2.8571428571428572</v>
       </c>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
@@ -7105,19 +7097,21 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="B11">
-        <v>32.14</v>
+        <f>MainDriver!B12</f>
+        <v>5000</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>9.81</v>
+        <v>4</v>
+      </c>
+      <c r="D11" s="45">
+        <f>B11*0.7457</f>
+        <v>3728.5</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
@@ -7129,837 +7123,863 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>32.14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>9.81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>15</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="49" t="s">
+      <c r="H14" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="49" t="s">
+      <c r="I14" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="J13" s="49" t="s">
+      <c r="J14" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="K13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
-        <v>0</v>
-      </c>
-      <c r="B14" s="45">
-        <f t="shared" ref="B14:B29" si="0">A14*$H$6*CFS_to_GPM</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="36">
-        <v>284.60390967860326</v>
-      </c>
-      <c r="D14" s="47">
-        <f t="shared" ref="D14:D29" si="1">100*C14*B14/(3960*E14)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="37">
-        <v>800</v>
-      </c>
-      <c r="F14" s="43"/>
-      <c r="G14">
-        <f t="shared" ref="G14:G29" si="2">A14*0.3048</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="49">
-        <f t="shared" ref="H14:H29" si="3">B14*0.0000630902</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="49">
-        <f t="shared" ref="I14:I29" si="4">C14*0.3048</f>
-        <v>86.747271670038273</v>
-      </c>
-      <c r="J14" s="50">
-        <f t="shared" ref="J14:J17" si="5">+E14*0.7457</f>
-        <v>596.56000000000006</v>
-      </c>
-      <c r="K14" s="2">
-        <f t="shared" ref="K14:K17" si="6">$D$11*H14*I14/J14</f>
+      <c r="K14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
+        <v>0</v>
+      </c>
+      <c r="B15" s="43">
+        <f t="shared" ref="B15:B30" si="0">A15*$H$6*CFS_to_GPM</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="36">
+        <v>284.60390967860326</v>
+      </c>
+      <c r="D15" s="13">
+        <f t="shared" ref="D15:D30" si="1">100*C15*B15/(3960*E15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="37">
+        <v>800</v>
+      </c>
+      <c r="F15" s="41"/>
+      <c r="G15">
+        <f t="shared" ref="G15:G30" si="2">A15*0.3048</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="45">
+        <f t="shared" ref="H15:H30" si="3">B15*0.0000630902</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="45">
+        <f t="shared" ref="I15:I30" si="4">C15*0.3048</f>
+        <v>86.747271670038273</v>
+      </c>
+      <c r="J15" s="46">
+        <f t="shared" ref="J15:J18" si="5">+E15*0.7457</f>
+        <v>596.56000000000006</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" ref="K15:K18" si="6">$D$12*H15*I15/J15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
         <v>2</v>
       </c>
-      <c r="B15" s="45">
+      <c r="B16" s="43">
         <f t="shared" si="0"/>
         <v>5659.760636050989</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C16" s="36">
         <v>283.63015918273595</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D16" s="13">
         <f t="shared" si="1"/>
         <v>32.799198934337774</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E16" s="37">
         <v>1235.9248093692947</v>
       </c>
-      <c r="F15" s="43"/>
-      <c r="G15">
+      <c r="F16" s="41"/>
+      <c r="G16">
         <f t="shared" si="2"/>
         <v>0.60960000000000003</v>
       </c>
-      <c r="H15" s="49">
+      <c r="H16" s="45">
         <f t="shared" si="3"/>
         <v>0.3570754304805841</v>
       </c>
-      <c r="I15" s="49">
+      <c r="I16" s="45">
         <f t="shared" si="4"/>
         <v>86.450472518897925</v>
       </c>
-      <c r="J15" s="50">
+      <c r="J16" s="46">
         <f t="shared" si="5"/>
         <v>921.62913034668316</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K16" s="2">
         <f t="shared" si="6"/>
         <v>0.32857926511540841</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="45">
+      <c r="B17" s="43">
         <f t="shared" si="0"/>
         <v>11319.521272101978</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C17" s="36">
         <v>282.32106151460493</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D17" s="13">
         <f t="shared" si="1"/>
         <v>44.591817117116321</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E17" s="37">
         <v>1809.7599877227742</v>
       </c>
-      <c r="F16" s="43"/>
-      <c r="G16">
+      <c r="F17" s="41"/>
+      <c r="G17">
         <f t="shared" si="2"/>
         <v>1.2192000000000001</v>
       </c>
-      <c r="H16" s="49">
+      <c r="H17" s="45">
         <f t="shared" si="3"/>
         <v>0.7141508609611682</v>
       </c>
-      <c r="I16" s="49">
+      <c r="I17" s="45">
         <f t="shared" si="4"/>
         <v>86.051459549651582</v>
       </c>
-      <c r="J16" s="50">
+      <c r="J17" s="46">
         <f t="shared" si="5"/>
         <v>1349.5380228448728</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K17" s="2">
         <f t="shared" si="6"/>
         <v>0.44671659597038255</v>
       </c>
     </row>
-    <row r="17" spans="1:25" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="39">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
         <v>6</v>
       </c>
-      <c r="B17" s="45">
+      <c r="B18" s="43">
         <f t="shared" si="0"/>
         <v>16979.281908152967</v>
       </c>
-      <c r="C17" s="46">
+      <c r="C18" s="36">
         <v>280.62143872503043</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D18" s="13">
         <f t="shared" si="1"/>
         <v>52.405097925520074</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E18" s="39">
         <v>2295.9976706516709</v>
       </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="41">
+      <c r="F18" s="42"/>
+      <c r="G18">
         <f t="shared" si="2"/>
         <v>1.8288000000000002</v>
       </c>
-      <c r="H17" s="51">
+      <c r="H18" s="45">
         <f t="shared" si="3"/>
         <v>1.0712262914417523</v>
       </c>
-      <c r="I17" s="51">
+      <c r="I18" s="45">
         <f t="shared" si="4"/>
         <v>85.533414523389283</v>
       </c>
-      <c r="J17" s="52">
+      <c r="J18" s="46">
         <f t="shared" si="5"/>
         <v>1712.1254630049511</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K18" s="40">
         <f t="shared" si="6"/>
         <v>0.52498930230400953</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
         <v>8</v>
       </c>
-      <c r="B18" s="45">
+      <c r="B19" s="43">
         <f t="shared" si="0"/>
         <v>22639.042544203956</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C19" s="36">
         <v>278.49043707319078</v>
       </c>
-      <c r="D18" s="47">
+      <c r="D19" s="13">
         <f t="shared" si="1"/>
         <v>58.217415029498866</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E19" s="38">
         <v>2734.7664193283617</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <f t="shared" si="2"/>
         <v>2.4384000000000001</v>
       </c>
-      <c r="H18" s="49">
+      <c r="H19" s="45">
         <f t="shared" si="3"/>
         <v>1.4283017219223364</v>
       </c>
-      <c r="I18" s="49">
+      <c r="I19" s="45">
         <f t="shared" si="4"/>
         <v>84.883885219908549</v>
       </c>
-      <c r="J18" s="50">
-        <f>+E18*0.7457</f>
+      <c r="J19" s="46">
+        <f>+E19*0.7457</f>
         <v>2039.3153188931594</v>
       </c>
-      <c r="K18" s="2">
-        <f>$D$11*H18*I18/J18</f>
+      <c r="K19" s="2">
+        <f t="shared" ref="K19:K27" si="7">$D$12*H19*I19/J19</f>
         <v>0.58321654396519762</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A20" s="6">
         <v>10</v>
       </c>
-      <c r="B19" s="45">
+      <c r="B20" s="43">
         <f t="shared" si="0"/>
         <v>28298.803180254945</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C20" s="36">
         <v>275.90201786958721</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D20" s="13">
         <f t="shared" si="1"/>
         <v>62.782468402691066</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E20" s="38">
         <v>3140.4318461172725</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <f t="shared" si="2"/>
         <v>3.048</v>
       </c>
-      <c r="H19" s="49">
+      <c r="H20" s="45">
         <f t="shared" si="3"/>
         <v>1.7853771524029203</v>
       </c>
-      <c r="I19" s="49">
+      <c r="I20" s="45">
         <f t="shared" si="4"/>
         <v>84.094935046650193</v>
       </c>
-      <c r="J19" s="49">
-        <f t="shared" ref="J19:J29" si="7">+E19*0.7457</f>
+      <c r="J20" s="45">
+        <f t="shared" ref="J20:J30" si="8">+E20*0.7457</f>
         <v>2341.82002764965</v>
       </c>
-      <c r="K19" s="2">
-        <f>$D$11*H19*I19/J19</f>
+      <c r="K20" s="2">
+        <f t="shared" si="7"/>
         <v>0.62894881582887918</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
         <v>12</v>
       </c>
-      <c r="B20" s="45">
+      <c r="B21" s="43">
         <f t="shared" si="0"/>
         <v>33958.563816305934</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C21" s="36">
         <v>272.84510084329219</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D21" s="13">
         <f t="shared" si="1"/>
         <v>66.475851600047918</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E21" s="38">
         <v>3519.7059244709994</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <f t="shared" si="2"/>
         <v>3.6576000000000004</v>
       </c>
-      <c r="H20" s="49">
+      <c r="H21" s="45">
         <f t="shared" si="3"/>
         <v>2.1424525828835046</v>
       </c>
-      <c r="I20" s="49">
+      <c r="I21" s="45">
         <f t="shared" si="4"/>
         <v>83.16318673703546</v>
       </c>
-      <c r="J20" s="49">
+      <c r="J21" s="45">
+        <f t="shared" si="8"/>
+        <v>2624.6447078780243</v>
+      </c>
+      <c r="K21" s="2">
         <f t="shared" si="7"/>
-        <v>2624.6447078780243</v>
-      </c>
-      <c r="K20" s="2">
-        <f>$D$11*H20*I20/J20</f>
         <v>0.66594877851719381</v>
       </c>
-      <c r="Y20">
+      <c r="Y21">
         <f>0.001797851/(0.00000001908315*2)</f>
         <v>47105.718919570405</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
         <v>14</v>
       </c>
-      <c r="B21" s="45">
+      <c r="B22" s="43">
         <f t="shared" si="0"/>
         <v>39618.324452356923</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C22" s="36">
         <v>269.32328822176822</v>
       </c>
-      <c r="D21" s="47">
+      <c r="D22" s="13">
         <f t="shared" si="1"/>
         <v>69.510253428598915</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E22" s="38">
         <v>3876.3765234392085</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <f t="shared" si="2"/>
         <v>4.2671999999999999</v>
       </c>
-      <c r="H21" s="49">
+      <c r="H22" s="45">
         <f t="shared" si="3"/>
         <v>2.4995280133640887</v>
       </c>
-      <c r="I21" s="49">
+      <c r="I22" s="45">
         <f t="shared" si="4"/>
         <v>82.089738249994952</v>
       </c>
-      <c r="J21" s="49">
+      <c r="J22" s="45">
+        <f t="shared" si="8"/>
+        <v>2890.6139735286179</v>
+      </c>
+      <c r="K22" s="2">
         <f t="shared" si="7"/>
-        <v>2890.6139735286179</v>
-      </c>
-      <c r="K21" s="2">
-        <f>$D$11*H21*I21/J21</f>
         <v>0.69634712833318069</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A22" s="6">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
         <v>16</v>
       </c>
-      <c r="B22" s="45">
+      <c r="B23" s="43">
         <f t="shared" si="0"/>
         <v>45278.085088407912</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C23" s="36">
         <v>265.35414000721357</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D23" s="13">
         <f t="shared" si="1"/>
         <v>72.014225198091921</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E23" s="38">
         <v>4213.087129155404</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <f t="shared" si="2"/>
         <v>4.8768000000000002</v>
       </c>
-      <c r="H22" s="49">
+      <c r="H23" s="45">
         <f t="shared" si="3"/>
         <v>2.8566034438446728</v>
       </c>
-      <c r="I22" s="49">
+      <c r="I23" s="45">
         <f t="shared" si="4"/>
         <v>80.879941874198707</v>
       </c>
-      <c r="J22" s="49">
+      <c r="J23" s="45">
+        <f t="shared" si="8"/>
+        <v>3141.699072211185</v>
+      </c>
+      <c r="K23" s="2">
         <f t="shared" si="7"/>
-        <v>3141.699072211185</v>
-      </c>
-      <c r="K22" s="2">
-        <f>$D$11*H22*I22/J22</f>
         <v>0.72143168010948622</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
         <v>18</v>
       </c>
-      <c r="B23" s="45">
+      <c r="B24" s="43">
         <f t="shared" si="0"/>
         <v>50937.845724458901</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C24" s="36">
         <v>260.96801410809252</v>
       </c>
-      <c r="D23" s="47">
+      <c r="D24" s="13">
         <f t="shared" si="1"/>
         <v>74.067569402059263</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E24" s="38">
         <v>4532.1531328549681</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <f t="shared" si="2"/>
         <v>5.4864000000000006</v>
       </c>
-      <c r="H23" s="49">
+      <c r="H24" s="45">
         <f t="shared" si="3"/>
         <v>3.2136788743252565</v>
       </c>
-      <c r="I23" s="49">
+      <c r="I24" s="45">
         <f t="shared" si="4"/>
         <v>79.543050700146608</v>
       </c>
-      <c r="J23" s="49">
+      <c r="J24" s="45">
+        <f t="shared" si="8"/>
+        <v>3379.6265911699497</v>
+      </c>
+      <c r="K24" s="2">
         <f t="shared" si="7"/>
-        <v>3379.6265911699497</v>
-      </c>
-      <c r="K23" s="2">
-        <f>$D$11*H23*I23/J23</f>
         <v>0.74200188765995889</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A25" s="6">
         <v>20</v>
       </c>
-      <c r="B24" s="45">
+      <c r="B25" s="43">
         <f t="shared" si="0"/>
         <v>56597.60636050989</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C25" s="36">
         <v>256.2065248654842</v>
       </c>
-      <c r="D24" s="47">
+      <c r="D25" s="13">
         <f t="shared" si="1"/>
         <v>75.719659588094515</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E25" s="38">
         <v>4835.9790562234675</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <f t="shared" si="2"/>
         <v>6.0960000000000001</v>
       </c>
-      <c r="H24" s="49">
+      <c r="H25" s="45">
         <f t="shared" si="3"/>
         <v>3.5707543048058406</v>
       </c>
-      <c r="I24" s="49">
+      <c r="I25" s="45">
         <f t="shared" si="4"/>
         <v>78.091748778999587</v>
       </c>
-      <c r="J24" s="49">
+      <c r="J25" s="45">
+        <f t="shared" si="8"/>
+        <v>3606.1895822258398</v>
+      </c>
+      <c r="K25" s="2">
         <f t="shared" si="7"/>
-        <v>3606.1895822258398</v>
-      </c>
-      <c r="K24" s="2">
-        <f>$D$11*H24*I24/J24</f>
         <v>0.75855237050310953</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A26" s="6">
         <v>22</v>
       </c>
-      <c r="B25" s="45">
+      <c r="B26" s="43">
         <f t="shared" si="0"/>
         <v>62257.366996560879</v>
       </c>
-      <c r="C25" s="36">
+      <c r="C26" s="36">
         <v>251.12070616305218</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D26" s="13">
         <f t="shared" si="1"/>
         <v>77.000062036058779</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E26" s="38">
         <v>5127.279735081358</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <f t="shared" si="2"/>
         <v>6.7056000000000004</v>
       </c>
-      <c r="H25" s="49">
+      <c r="H26" s="45">
         <f t="shared" si="3"/>
         <v>3.9278297352864247</v>
       </c>
-      <c r="I25" s="49">
+      <c r="I26" s="45">
         <f t="shared" si="4"/>
         <v>76.541591238498313</v>
       </c>
-      <c r="J25" s="49">
+      <c r="J26" s="45">
+        <f t="shared" si="8"/>
+        <v>3823.4124984501686</v>
+      </c>
+      <c r="K26" s="2">
         <f t="shared" si="7"/>
-        <v>3823.4124984501686</v>
-      </c>
-      <c r="K25" s="2">
-        <f>$D$11*H25*I25/J25</f>
         <v>0.77137932082730243</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A27" s="6">
         <v>24</v>
       </c>
-      <c r="B26" s="45">
+      <c r="B27" s="43">
         <f t="shared" si="0"/>
         <v>67917.127632611868</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C27" s="36">
         <v>245.76898773308471</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D27" s="13">
         <f t="shared" si="1"/>
         <v>77.925349887089979</v>
       </c>
-      <c r="E26" s="38">
+      <c r="E27" s="38">
         <v>5409.1925870129789</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <f t="shared" si="2"/>
         <v>7.3152000000000008</v>
       </c>
-      <c r="H26" s="49">
+      <c r="H27" s="45">
         <f t="shared" si="3"/>
         <v>4.2849051657670092</v>
       </c>
-      <c r="I26" s="49">
+      <c r="I27" s="45">
         <f t="shared" si="4"/>
         <v>74.910387461044223</v>
       </c>
-      <c r="J26" s="49">
+      <c r="J27" s="45">
+        <f t="shared" si="8"/>
+        <v>4033.6349121355784</v>
+      </c>
+      <c r="K27" s="2">
         <f t="shared" si="7"/>
-        <v>4033.6349121355784</v>
-      </c>
-      <c r="K26" s="2">
-        <f>$D$11*H26*I26/J26</f>
         <v>0.78064876678909856</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A28" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="45">
+      <c r="B28" s="43">
         <f t="shared" si="0"/>
         <v>73576.888268662864</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C28" s="36">
         <v>240.21510391176363</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D28" s="13">
         <f t="shared" si="1"/>
         <v>78.503908610427686</v>
       </c>
-      <c r="E27" s="38">
+      <c r="E28" s="38">
         <v>5685.3245450995701</v>
       </c>
-      <c r="G27">
+      <c r="G28">
         <f t="shared" si="2"/>
         <v>7.9248000000000003</v>
       </c>
-      <c r="H27" s="49">
+      <c r="H28" s="45">
         <f t="shared" si="3"/>
         <v>4.6419805962475937</v>
       </c>
-      <c r="I27" s="49">
+      <c r="I28" s="45">
         <f t="shared" si="4"/>
         <v>73.217563672305559</v>
       </c>
-      <c r="J27" s="49">
-        <f t="shared" si="7"/>
+      <c r="J28" s="45">
+        <f t="shared" si="8"/>
         <v>4239.5465132807494</v>
       </c>
-      <c r="K27" s="2">
-        <f t="shared" ref="K27" si="8">$D$11*H27*I27/J27</f>
+      <c r="K28" s="2">
+        <f t="shared" ref="K28" si="9">$D$12*H28*I28/J28</f>
         <v>0.786444713224284</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B28" s="45">
+      <c r="B29" s="43">
         <f t="shared" si="0"/>
         <v>79236.648904713846</v>
       </c>
-      <c r="C28" s="36">
+      <c r="C29" s="36">
         <v>234.52605302036019</v>
       </c>
-      <c r="D28" s="47">
+      <c r="D29" s="13">
         <f t="shared" si="1"/>
         <v>78.739626218925864</v>
       </c>
-      <c r="E28" s="38">
+      <c r="E29" s="38">
         <v>5959.7584740347256</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <f t="shared" si="2"/>
         <v>8.5343999999999998</v>
       </c>
-      <c r="H28" s="49">
+      <c r="H29" s="45">
         <f t="shared" si="3"/>
         <v>4.9990560267281774</v>
       </c>
-      <c r="I28" s="49">
+      <c r="I29" s="45">
         <f t="shared" si="4"/>
         <v>71.483540960605794</v>
       </c>
-      <c r="J28" s="49">
-        <f t="shared" si="7"/>
+      <c r="J29" s="45">
+        <f t="shared" si="8"/>
         <v>4444.1918940876949</v>
       </c>
-      <c r="K28" s="2">
-        <f>$D$11*H28*I28/J28</f>
+      <c r="K29" s="2">
+        <f>$D$12*H29*I29/J29</f>
         <v>0.78880610987699351</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A30" s="6">
         <v>30</v>
       </c>
-      <c r="B29" s="45">
+      <c r="B30" s="43">
         <f t="shared" si="0"/>
         <v>84896.409540764827</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C30" s="36">
         <v>228.77021431529786</v>
       </c>
-      <c r="D29" s="47">
+      <c r="D30" s="13">
         <f t="shared" si="1"/>
         <v>78.634926058357621</v>
       </c>
-      <c r="E29" s="38">
+      <c r="E30" s="38">
         <v>6237.0343184602061</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <f t="shared" si="2"/>
         <v>9.1440000000000001</v>
       </c>
-      <c r="H29" s="49">
+      <c r="H30" s="45">
         <f t="shared" si="3"/>
         <v>5.356131457208761</v>
       </c>
-      <c r="I29" s="49">
+      <c r="I30" s="45">
         <f t="shared" si="4"/>
         <v>69.72916132330279</v>
       </c>
-      <c r="J29" s="49">
-        <f t="shared" si="7"/>
+      <c r="J30" s="45">
+        <f t="shared" si="8"/>
         <v>4650.956491275776</v>
       </c>
-      <c r="K29" s="2">
-        <f>$D$11*H29*I29/J29</f>
+      <c r="K30" s="2">
+        <f>$D$12*H30*I30/J30</f>
         <v>0.78775723359541561</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="K30" s="2"/>
-    </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="H31" t="str">
-        <f>TEXT(H14,"0.0000000")&amp;": "&amp;TEXT(I14,"0.000000")&amp;","</f>
-        <v>0.0000000: 86.747272,</v>
-      </c>
-      <c r="J31" t="str">
-        <f>TEXT(H14,"0.000000")&amp;": "&amp;TEXT(J14,"0.000000")&amp;","</f>
-        <v>0.000000: 596.560000,</v>
-      </c>
+      <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="H32" t="str">
-        <f>TEXT(H15,"0.0000000")&amp;": "&amp;TEXT(I15,"0.000000")&amp;","</f>
-        <v>0.3570754: 86.450473,</v>
+        <f t="shared" ref="H32:H47" si="10">TEXT(H15,"0.0000000")&amp;": "&amp;TEXT(I15,"0.000000")&amp;","</f>
+        <v>0.0000000: 86.747272,</v>
       </c>
       <c r="J32" t="str">
-        <f>TEXT(H15,"0.000000")&amp;": "&amp;TEXT(J15,"0.000000")&amp;","</f>
-        <v>0.357075: 921.629130,</v>
+        <f t="shared" ref="J32:J47" si="11">TEXT(H15,"0.000000")&amp;": "&amp;TEXT(J15,"0.000000")&amp;","</f>
+        <v>0.000000: 596.560000,</v>
       </c>
     </row>
     <row r="33" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H33" t="str">
-        <f>TEXT(H16,"0.0000000")&amp;": "&amp;TEXT(I16,"0.000000")&amp;","</f>
-        <v>0.7141509: 86.051460,</v>
+        <f t="shared" si="10"/>
+        <v>0.3570754: 86.450473,</v>
       </c>
       <c r="J33" t="str">
-        <f>TEXT(H16,"0.000000")&amp;": "&amp;TEXT(J16,"0.000000")&amp;","</f>
-        <v>0.714151: 1349.538023,</v>
+        <f t="shared" si="11"/>
+        <v>0.357075: 921.629130,</v>
       </c>
     </row>
     <row r="34" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H34" t="str">
-        <f>TEXT(H17,"0.0000000")&amp;": "&amp;TEXT(I17,"0.000000")&amp;","</f>
-        <v>1.0712263: 85.533415,</v>
+        <f t="shared" si="10"/>
+        <v>0.7141509: 86.051460,</v>
       </c>
       <c r="J34" t="str">
-        <f>TEXT(H17,"0.000000")&amp;": "&amp;TEXT(J17,"0.000000")&amp;","</f>
-        <v>1.071226: 1712.125463,</v>
+        <f t="shared" si="11"/>
+        <v>0.714151: 1349.538023,</v>
       </c>
     </row>
     <row r="35" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H35" t="str">
-        <f>TEXT(H18,"0.0000000")&amp;": "&amp;TEXT(I18,"0.000000")&amp;","</f>
-        <v>1.4283017: 84.883885,</v>
+        <f t="shared" si="10"/>
+        <v>1.0712263: 85.533415,</v>
       </c>
       <c r="J35" t="str">
-        <f>TEXT(H18,"0.000000")&amp;": "&amp;TEXT(J18,"0.000000")&amp;","</f>
-        <v>1.428302: 2039.315319,</v>
+        <f t="shared" si="11"/>
+        <v>1.071226: 1712.125463,</v>
       </c>
     </row>
     <row r="36" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H36" t="str">
-        <f>TEXT(H19,"0.0000000")&amp;": "&amp;TEXT(I19,"0.000000")&amp;","</f>
-        <v>1.7853772: 84.094935,</v>
+        <f t="shared" si="10"/>
+        <v>1.4283017: 84.883885,</v>
       </c>
       <c r="J36" t="str">
-        <f>TEXT(H19,"0.000000")&amp;": "&amp;TEXT(J19,"0.000000")&amp;","</f>
-        <v>1.785377: 2341.820028,</v>
+        <f t="shared" si="11"/>
+        <v>1.428302: 2039.315319,</v>
       </c>
     </row>
     <row r="37" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H37" t="str">
-        <f>TEXT(H20,"0.0000000")&amp;": "&amp;TEXT(I20,"0.000000")&amp;","</f>
-        <v>2.1424526: 83.163187,</v>
+        <f t="shared" si="10"/>
+        <v>1.7853772: 84.094935,</v>
       </c>
       <c r="J37" t="str">
-        <f>TEXT(H20,"0.000000")&amp;": "&amp;TEXT(J20,"0.000000")&amp;","</f>
-        <v>2.142453: 2624.644708,</v>
+        <f t="shared" si="11"/>
+        <v>1.785377: 2341.820028,</v>
       </c>
     </row>
     <row r="38" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H38" t="str">
-        <f>TEXT(H21,"0.0000000")&amp;": "&amp;TEXT(I21,"0.000000")&amp;","</f>
-        <v>2.4995280: 82.089738,</v>
+        <f t="shared" si="10"/>
+        <v>2.1424526: 83.163187,</v>
       </c>
       <c r="J38" t="str">
-        <f>TEXT(H21,"0.000000")&amp;": "&amp;TEXT(J21,"0.000000")&amp;","</f>
-        <v>2.499528: 2890.613974,</v>
+        <f t="shared" si="11"/>
+        <v>2.142453: 2624.644708,</v>
       </c>
     </row>
     <row r="39" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H39" t="str">
-        <f>TEXT(H22,"0.0000000")&amp;": "&amp;TEXT(I22,"0.000000")&amp;","</f>
-        <v>2.8566034: 80.879942,</v>
+        <f t="shared" si="10"/>
+        <v>2.4995280: 82.089738,</v>
       </c>
       <c r="J39" t="str">
-        <f>TEXT(H22,"0.000000")&amp;": "&amp;TEXT(J22,"0.000000")&amp;","</f>
-        <v>2.856603: 3141.699072,</v>
+        <f t="shared" si="11"/>
+        <v>2.499528: 2890.613974,</v>
       </c>
     </row>
     <row r="40" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H40" t="str">
-        <f>TEXT(H23,"0.0000000")&amp;": "&amp;TEXT(I23,"0.000000")&amp;","</f>
-        <v>3.2136789: 79.543051,</v>
+        <f t="shared" si="10"/>
+        <v>2.8566034: 80.879942,</v>
       </c>
       <c r="J40" t="str">
-        <f>TEXT(H23,"0.000000")&amp;": "&amp;TEXT(J23,"0.000000")&amp;","</f>
-        <v>3.213679: 3379.626591,</v>
+        <f t="shared" si="11"/>
+        <v>2.856603: 3141.699072,</v>
       </c>
     </row>
     <row r="41" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H41" t="str">
-        <f>TEXT(H24,"0.0000000")&amp;": "&amp;TEXT(I24,"0.000000")&amp;","</f>
-        <v>3.5707543: 78.091749,</v>
+        <f t="shared" si="10"/>
+        <v>3.2136789: 79.543051,</v>
       </c>
       <c r="J41" t="str">
-        <f>TEXT(H24,"0.000000")&amp;": "&amp;TEXT(J24,"0.000000")&amp;","</f>
-        <v>3.570754: 3606.189582,</v>
+        <f t="shared" si="11"/>
+        <v>3.213679: 3379.626591,</v>
       </c>
     </row>
     <row r="42" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H42" t="str">
-        <f>TEXT(H25,"0.0000000")&amp;": "&amp;TEXT(I25,"0.000000")&amp;","</f>
-        <v>3.9278297: 76.541591,</v>
+        <f t="shared" si="10"/>
+        <v>3.5707543: 78.091749,</v>
       </c>
       <c r="J42" t="str">
-        <f>TEXT(H25,"0.000000")&amp;": "&amp;TEXT(J25,"0.000000")&amp;","</f>
-        <v>3.927830: 3823.412498,</v>
+        <f t="shared" si="11"/>
+        <v>3.570754: 3606.189582,</v>
       </c>
     </row>
     <row r="43" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H43" t="str">
-        <f>TEXT(H26,"0.0000000")&amp;": "&amp;TEXT(I26,"0.000000")&amp;","</f>
-        <v>4.2849052: 74.910387,</v>
+        <f t="shared" si="10"/>
+        <v>3.9278297: 76.541591,</v>
       </c>
       <c r="J43" t="str">
-        <f>TEXT(H26,"0.000000")&amp;": "&amp;TEXT(J26,"0.000000")&amp;","</f>
-        <v>4.284905: 4033.634912,</v>
+        <f t="shared" si="11"/>
+        <v>3.927830: 3823.412498,</v>
       </c>
     </row>
     <row r="44" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H44" t="str">
-        <f>TEXT(H27,"0.0000000")&amp;": "&amp;TEXT(I27,"0.000000")&amp;","</f>
-        <v>4.6419806: 73.217564,</v>
+        <f t="shared" si="10"/>
+        <v>4.2849052: 74.910387,</v>
       </c>
       <c r="J44" t="str">
-        <f>TEXT(H27,"0.000000")&amp;": "&amp;TEXT(J27,"0.000000")&amp;","</f>
-        <v>4.641981: 4239.546513,</v>
+        <f t="shared" si="11"/>
+        <v>4.284905: 4033.634912,</v>
       </c>
     </row>
     <row r="45" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H45" t="str">
-        <f>TEXT(H28,"0.0000000")&amp;": "&amp;TEXT(I28,"0.000000")&amp;","</f>
-        <v>4.9990560: 71.483541,</v>
+        <f t="shared" si="10"/>
+        <v>4.6419806: 73.217564,</v>
       </c>
       <c r="J45" t="str">
-        <f>TEXT(H28,"0.000000")&amp;": "&amp;TEXT(J28,"0.000000")&amp;","</f>
-        <v>4.999056: 4444.191894,</v>
+        <f t="shared" si="11"/>
+        <v>4.641981: 4239.546513,</v>
       </c>
     </row>
     <row r="46" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H46" t="str">
-        <f>TEXT(H29,"0.0000000")&amp;": "&amp;TEXT(I29,"0.000000")&amp;","</f>
+        <f t="shared" si="10"/>
+        <v>4.9990560: 71.483541,</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="11"/>
+        <v>4.999056: 4444.191894,</v>
+      </c>
+    </row>
+    <row r="47" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H47" t="str">
+        <f t="shared" si="10"/>
         <v>5.3561315: 69.729161,</v>
       </c>
-      <c r="J46" t="str">
-        <f>TEXT(H29,"0.000000")&amp;": "&amp;TEXT(J29,"0.000000")&amp;","</f>
+      <c r="J47" t="str">
+        <f t="shared" si="11"/>
         <v>5.356131: 4650.956491,</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>$B$10/$B$11</formula>
+      <formula>$B$11/$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7971,10 +7991,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B313AEA-B752-4529-9A71-63CCB4B8A2E8}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7989,173 +8009,164 @@
       <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="49">
-        <f>A14/MainPump!B7</f>
-        <v>2.8571428571428572</v>
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="B4" s="35">
+        <v>700.00000000000011</v>
+      </c>
+      <c r="D4" s="49">
+        <f>A4/60</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E4" s="50">
+        <f>B4*0.7457</f>
+        <v>521.99000000000012</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="49" t="s">
-        <v>24</v>
+      <c r="A5">
+        <v>300</v>
+      </c>
+      <c r="B5" s="35">
+        <v>950</v>
+      </c>
+      <c r="D5" s="49">
+        <f t="shared" ref="D5:D12" si="0">A5/60</f>
+        <v>5</v>
+      </c>
+      <c r="E5" s="50">
+        <f t="shared" ref="E5:E12" si="1">B5*0.7457</f>
+        <v>708.41500000000008</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="B6" s="35">
-        <v>700.00000000000011</v>
-      </c>
-      <c r="D6" s="55">
-        <f>A6/60</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="E6" s="56">
-        <f>B6*0.7457</f>
-        <v>521.99000000000012</v>
+        <v>1450</v>
+      </c>
+      <c r="D6" s="49">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E6" s="50">
+        <f t="shared" si="1"/>
+        <v>1081.2650000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="B7" s="35">
-        <v>950</v>
-      </c>
-      <c r="D7" s="55">
-        <f t="shared" ref="D7:D14" si="0">A7/60</f>
-        <v>5</v>
-      </c>
-      <c r="E7" s="56">
-        <f t="shared" ref="E7:E14" si="1">B7*0.7457</f>
-        <v>708.41500000000008</v>
+        <v>2250</v>
+      </c>
+      <c r="D7" s="49">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="E7" s="50">
+        <f t="shared" si="1"/>
+        <v>1677.825</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="B8" s="35">
-        <v>1450</v>
-      </c>
-      <c r="D8" s="55">
+        <v>3200</v>
+      </c>
+      <c r="D8" s="49">
         <f t="shared" si="0"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="E8" s="56">
+        <v>10</v>
+      </c>
+      <c r="E8" s="50">
         <f t="shared" si="1"/>
-        <v>1081.2650000000001</v>
+        <v>2386.2400000000002</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="B9" s="35">
-        <v>2250</v>
-      </c>
-      <c r="D9" s="55">
+        <v>4400</v>
+      </c>
+      <c r="D9" s="49">
         <f t="shared" si="0"/>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="E9" s="56">
+        <v>11.666666666666666</v>
+      </c>
+      <c r="E9" s="50">
         <f t="shared" si="1"/>
-        <v>1677.825</v>
+        <v>3281.08</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>600</v>
+        <v>765</v>
       </c>
       <c r="B10" s="35">
-        <v>3200</v>
-      </c>
-      <c r="D10" s="55">
+        <v>4850</v>
+      </c>
+      <c r="D10" s="49">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="E10" s="56">
+        <v>12.75</v>
+      </c>
+      <c r="E10" s="50">
         <f t="shared" si="1"/>
-        <v>2386.2400000000002</v>
+        <v>3616.645</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="B11" s="35">
-        <v>4400</v>
-      </c>
-      <c r="D11" s="55">
+        <v>5000</v>
+      </c>
+      <c r="D11" s="49">
         <f t="shared" si="0"/>
-        <v>11.666666666666666</v>
-      </c>
-      <c r="E11" s="56">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="E11" s="50">
         <f t="shared" si="1"/>
-        <v>3281.08</v>
+        <v>3728.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>765</v>
+        <v>900</v>
       </c>
       <c r="B12" s="35">
-        <v>4850</v>
-      </c>
-      <c r="D12" s="55">
-        <f t="shared" si="0"/>
-        <v>12.75</v>
-      </c>
-      <c r="E12" s="56">
-        <f t="shared" si="1"/>
-        <v>3616.645</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>800</v>
-      </c>
-      <c r="B13" s="35">
         <v>5000</v>
       </c>
-      <c r="D13" s="55">
-        <f t="shared" si="0"/>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="E13" s="56">
-        <f t="shared" si="1"/>
-        <v>3728.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>900</v>
-      </c>
-      <c r="B14" s="35">
-        <v>5000</v>
-      </c>
-      <c r="D14" s="55">
+      <c r="D12" s="49">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E14" s="56">
+      <c r="E12" s="50">
         <f t="shared" si="1"/>
         <v>3728.5</v>
       </c>

</xml_diff>

<commit_message>
Load a pipeline from the workbook
</commit_message>
<xml_diff>
--- a/DHLLDV_viewer/static/pipelines/Example_input.xlsx
+++ b/DHLLDV_viewer/static/pipelines/Example_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcrii\PycharmProjects\DHLLDV\DHLLDV_viewer\static\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934B4C02-F6F0-4E14-A58E-FE443B548A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E07A3FB-9BDA-4319-BA08-60216280C34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipeline" sheetId="11" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <definedName name="name" localSheetId="2">MainPump!$B$2</definedName>
     <definedName name="name" localSheetId="0">Pipeline!$B$1</definedName>
     <definedName name="name" localSheetId="1">UWPump!$B$2</definedName>
+    <definedName name="pipe_table" localSheetId="0">Pipeline!$A$21:$F$32</definedName>
     <definedName name="power_curve" localSheetId="3">MainDriver!$D$3:$E$12</definedName>
     <definedName name="pump_curve" localSheetId="2">MainPump!$H$14:$J$30</definedName>
     <definedName name="pump_curve" localSheetId="1">UWPump!$H$14:$J$30</definedName>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t>Eff</t>
   </si>
@@ -244,27 +245,15 @@
     <t>Dig Depth</t>
   </si>
   <si>
-    <t>Dia (m)</t>
-  </si>
-  <si>
     <t>Dredge Discharge</t>
   </si>
   <si>
-    <t>Main Pump</t>
-  </si>
-  <si>
     <t>copy.copy(Ladder_Pump),</t>
   </si>
   <si>
     <t>copy.copy(Main_Pump),</t>
   </si>
   <si>
-    <t>Len (m)</t>
-  </si>
-  <si>
-    <t>delta Z (m)</t>
-  </si>
-  <si>
     <t>Final Elev (m)</t>
   </si>
   <si>
@@ -311,6 +300,27 @@
   </si>
   <si>
     <t>torque</t>
+  </si>
+  <si>
+    <t>Pipe Name</t>
+  </si>
+  <si>
+    <t>Diameter (m)</t>
+  </si>
+  <si>
+    <t>Length (m)</t>
+  </si>
+  <si>
+    <t>UWPump</t>
+  </si>
+  <si>
+    <t>MainPump</t>
+  </si>
+  <si>
+    <t>Total K</t>
+  </si>
+  <si>
+    <t>Elev Change (m)</t>
   </si>
 </sst>
 </file>
@@ -4795,23 +4805,25 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -5415,22 +5427,22 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
@@ -5526,7 +5538,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B24" s="32"/>
       <c r="C24" s="24"/>
@@ -5537,7 +5549,7 @@
         <v>-11.5824</v>
       </c>
       <c r="G24" s="34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -5633,7 +5645,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="24"/>
@@ -5643,7 +5655,7 @@
         <v>10</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -5659,7 +5671,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="31">
         <f>(B11/12)*0.3048</f>
@@ -5888,7 +5900,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -5922,7 +5934,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" s="6">
         <v>60</v>
@@ -5940,7 +5952,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B5" s="6">
         <v>34</v>
@@ -5958,7 +5970,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B6" s="6">
         <v>34</v>
@@ -5986,7 +5998,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B7" s="6">
         <v>300</v>
@@ -6015,10 +6027,10 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -6040,7 +6052,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B11">
         <v>2000</v>
@@ -6111,10 +6123,10 @@
         <v>12</v>
       </c>
       <c r="H14" s="45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J14" s="45" t="s">
         <v>24</v>
@@ -6964,12 +6976,12 @@
         <v>21</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" s="6">
         <v>84</v>
@@ -6987,7 +6999,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B5" s="6">
         <v>34</v>
@@ -7005,7 +7017,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B6" s="6">
         <v>34</v>
@@ -7033,7 +7045,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B7" s="6">
         <v>315</v>
@@ -7062,10 +7074,10 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -7097,7 +7109,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B11">
         <f>MainDriver!B12</f>
@@ -7169,10 +7181,10 @@
         <v>12</v>
       </c>
       <c r="H14" s="45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J14" s="45" t="s">
         <v>24</v>
@@ -7994,7 +8006,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8010,7 +8022,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -8021,7 +8033,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E3" s="45" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Load the slurry from the workbook and apply to the pipeline
</commit_message>
<xml_diff>
--- a/DHLLDV_viewer/static/pipelines/Example_input.xlsx
+++ b/DHLLDV_viewer/static/pipelines/Example_input.xlsx
@@ -8,27 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcrii\PycharmProjects\DHLLDV\DHLLDV_viewer\static\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E07A3FB-9BDA-4319-BA08-60216280C34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97485615-0AA0-4303-93AB-8A2724E94D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipeline" sheetId="11" r:id="rId1"/>
     <sheet name="UWPump" sheetId="14" r:id="rId2"/>
     <sheet name="MainPump" sheetId="12" r:id="rId3"/>
     <sheet name="MainDriver" sheetId="13" r:id="rId4"/>
+    <sheet name="Slurry" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="avail_power" localSheetId="2">MainPump!$D$11</definedName>
     <definedName name="avail_power" localSheetId="1">UWPump!$D$11</definedName>
     <definedName name="CFS_to_GPM" localSheetId="2">MainPump!$I$1</definedName>
     <definedName name="CFS_to_GPM" localSheetId="1">UWPump!$I$1</definedName>
+    <definedName name="Cv" localSheetId="4">Slurry!$C$10</definedName>
+    <definedName name="d_15" localSheetId="4">Slurry!$C$5</definedName>
+    <definedName name="d_50" localSheetId="4">Slurry!$C$6</definedName>
+    <definedName name="d_85" localSheetId="4">Slurry!$C$7</definedName>
     <definedName name="design_impeller" localSheetId="2">MainPump!$D$4</definedName>
     <definedName name="design_impeller" localSheetId="1">UWPump!$D$4</definedName>
     <definedName name="design_speed" localSheetId="2">MainPump!$D$7</definedName>
     <definedName name="design_speed" localSheetId="1">UWPump!$D$7</definedName>
     <definedName name="disch_dia" localSheetId="2">MainPump!$D$6</definedName>
     <definedName name="disch_dia" localSheetId="1">UWPump!$D$6</definedName>
+    <definedName name="fluid" localSheetId="4">Slurry!$C$9</definedName>
     <definedName name="gear_ratio" localSheetId="2">MainPump!$D$10</definedName>
     <definedName name="gear_ratio" localSheetId="1">UWPump!$D$10</definedName>
     <definedName name="limited" localSheetId="2">MainPump!$D$9</definedName>
@@ -36,11 +42,15 @@
     <definedName name="name" localSheetId="3">MainDriver!$B$1</definedName>
     <definedName name="name" localSheetId="2">MainPump!$B$2</definedName>
     <definedName name="name" localSheetId="0">Pipeline!$B$1</definedName>
+    <definedName name="name" localSheetId="4">Slurry!$C$1</definedName>
     <definedName name="name" localSheetId="1">UWPump!$B$2</definedName>
+    <definedName name="pipe_dia" localSheetId="4">Slurry!$C$3</definedName>
     <definedName name="pipe_table" localSheetId="0">Pipeline!$A$21:$F$32</definedName>
     <definedName name="power_curve" localSheetId="3">MainDriver!$D$3:$E$12</definedName>
     <definedName name="pump_curve" localSheetId="2">MainPump!$H$14:$J$30</definedName>
     <definedName name="pump_curve" localSheetId="1">UWPump!$H$14:$J$30</definedName>
+    <definedName name="rhoi" localSheetId="4">Slurry!$C$13</definedName>
+    <definedName name="rhos" localSheetId="4">Slurry!$C$12</definedName>
     <definedName name="suction_dia" localSheetId="2">MainPump!$D$5</definedName>
     <definedName name="suction_dia" localSheetId="1">UWPump!$D$5</definedName>
   </definedNames>
@@ -63,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="101">
   <si>
     <t>Eff</t>
   </si>
@@ -321,6 +331,51 @@
   </si>
   <si>
     <t>Elev Change (m)</t>
+  </si>
+  <si>
+    <t>Slurry Name:</t>
+  </si>
+  <si>
+    <t>Pipe Dia:</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>D50</t>
+  </si>
+  <si>
+    <t>D85</t>
+  </si>
+  <si>
+    <t>fluid</t>
+  </si>
+  <si>
+    <t>Cv</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>rhos</t>
+  </si>
+  <si>
+    <t>rhoi</t>
+  </si>
+  <si>
+    <t>ton/m3</t>
+  </si>
+  <si>
+    <t>salt or fresh</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>F Sand</t>
+  </si>
+  <si>
+    <t>salt</t>
   </si>
 </sst>
 </file>
@@ -459,7 +514,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -540,6 +595,10 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -4805,7 +4864,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -8187,4 +8246,119 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D933E8-A59A-4E9F-B033-19382DFDA4BB}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="6">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="53">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="53">
+        <v>1.92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix pump names in US-Units section & copy names from US to SI units section
Did not look like it followed the rules
</commit_message>
<xml_diff>
--- a/DHLLDV_viewer/static/pipelines/Example_input.xlsx
+++ b/DHLLDV_viewer/static/pipelines/Example_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcrii\PycharmProjects\DHLLDV\DHLLDV_viewer\static\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8A3F1A-7ACF-4A4A-A052-3065091C3511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD11B7B-3BE1-43DF-965A-E643421BD784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{36A6D056-07A8-4E30-AFB9-7896CA916417}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipeline" sheetId="11" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="95">
   <si>
     <t>Eff</t>
   </si>
@@ -177,9 +177,6 @@
     <t>MP 2 Discharge</t>
   </si>
   <si>
-    <t>Main Pump 1</t>
-  </si>
-  <si>
     <t>CL</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
     <t>UWP to Trunion</t>
   </si>
   <si>
-    <t>Underwater Pump</t>
-  </si>
-  <si>
     <t>UWP Suction</t>
   </si>
   <si>
@@ -250,9 +244,6 @@
   </si>
   <si>
     <t>Dig Depth</t>
-  </si>
-  <si>
-    <t>Dredge Discharge</t>
   </si>
   <si>
     <t>Final Elev (m)</t>
@@ -499,7 +490,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -599,10 +590,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4872,8 +4862,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4887,22 +4877,22 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="67">
+        <v>56</v>
+      </c>
+      <c r="C3" s="66">
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H3" s="9">
         <v>0.19</v>
@@ -4943,34 +4933,34 @@
     </row>
     <row r="4" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H4" s="10">
         <v>90</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K4" s="10">
         <v>45</v>
@@ -4982,27 +4972,27 @@
         <v>15</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4">
         <v>34</v>
@@ -5035,7 +5025,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="25">
         <v>34</v>
@@ -5047,7 +5037,7 @@
         <f t="shared" ref="D6:D15" si="0">SUMPRODUCT(H6:S6,H$2:S$2)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="66">
+      <c r="E6" s="11">
         <f>(F10-E5)*C6/(C6+C8)</f>
         <v>12</v>
       </c>
@@ -5070,7 +5060,7 @@
     </row>
     <row r="7" spans="1:19" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25">
@@ -5080,7 +5070,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E7" s="66"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="20">
         <f>F6</f>
         <v>-38</v>
@@ -5100,7 +5090,7 @@
     </row>
     <row r="8" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="25">
         <v>34</v>
@@ -5112,7 +5102,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" s="66">
+      <c r="E8" s="11">
         <f>(F10-F5)-E6</f>
         <v>48</v>
       </c>
@@ -5121,7 +5111,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="16">
         <v>1</v>
@@ -5141,7 +5131,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="25">
         <v>34</v>
@@ -5161,7 +5151,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5179,7 +5169,7 @@
     </row>
     <row r="10" spans="1:19" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="25">
@@ -5472,7 +5462,7 @@
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20">
         <f>C3*0.3048</f>
@@ -5495,22 +5485,22 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="43" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C21" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="44" t="s">
-        <v>81</v>
-      </c>
       <c r="E21" s="44" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F21" s="44" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -5525,8 +5515,9 @@
       <c r="S21" s="9"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="45" t="s">
-        <v>41</v>
+      <c r="A22" s="45" t="str">
+        <f>A5</f>
+        <v>Entrance</v>
       </c>
       <c r="B22" s="46">
         <f>(B5/12)*0.3048</f>
@@ -5561,23 +5552,24 @@
       <c r="S22" s="9"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="34" t="s">
-        <v>40</v>
+      <c r="A23" s="34" t="str">
+        <f t="shared" ref="A23:A32" si="2">A6</f>
+        <v>UWP Suction</v>
       </c>
       <c r="B23" s="40">
         <f>(B6/12)*0.3048</f>
         <v>0.86360000000000003</v>
       </c>
       <c r="C23" s="34">
-        <f t="shared" ref="C23:C32" si="2">C6*0.3048</f>
+        <f t="shared" ref="C23:C32" si="3">C6*0.3048</f>
         <v>4.5720000000000001</v>
       </c>
       <c r="D23" s="38">
-        <f t="shared" ref="D23:D32" si="3">D6</f>
+        <f t="shared" ref="D23:D32" si="4">D6</f>
         <v>0</v>
       </c>
       <c r="E23" s="49">
-        <f t="shared" ref="E23:E32" si="4">E6*0.3048</f>
+        <f t="shared" ref="E23:E32" si="5">E6*0.3048</f>
         <v>3.6576000000000004</v>
       </c>
       <c r="F23" s="49">
@@ -5597,15 +5589,16 @@
       <c r="S23" s="9"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="50" t="s">
-        <v>79</v>
+      <c r="A24" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v>UWPump</v>
       </c>
       <c r="B24" s="51"/>
       <c r="C24" s="52"/>
       <c r="D24" s="53"/>
       <c r="E24" s="52"/>
       <c r="F24" s="52">
-        <f t="shared" ref="F24:F32" si="5">F23+E24</f>
+        <f t="shared" ref="F24:F32" si="6">F23+E24</f>
         <v>-11.5824</v>
       </c>
       <c r="G24" s="24"/>
@@ -5622,27 +5615,28 @@
       <c r="S24" s="9"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="45" t="s">
-        <v>38</v>
+      <c r="A25" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>UWP to Trunion</v>
       </c>
       <c r="B25" s="46">
         <f>(B8/12)*0.3048</f>
         <v>0.86360000000000003</v>
       </c>
       <c r="C25" s="54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.288</v>
       </c>
       <c r="D25" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E25" s="54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.630400000000002</v>
       </c>
       <c r="F25" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.0480000000000018</v>
       </c>
       <c r="H25" s="9"/>
@@ -5658,27 +5652,28 @@
       <c r="S25" s="9"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="34" t="s">
-        <v>36</v>
+      <c r="A26" s="34" t="str">
+        <f t="shared" si="2"/>
+        <v>MP 1 Suction</v>
       </c>
       <c r="B26" s="40">
         <f>(B9/12)*0.3048</f>
         <v>0.86360000000000003</v>
       </c>
       <c r="C26" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.048</v>
       </c>
       <c r="D26" s="38">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="49">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="E26" s="49">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="F26" s="49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.0480000000000018</v>
       </c>
       <c r="H26" s="9"/>
@@ -5694,15 +5689,16 @@
       <c r="S26" s="9"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="50" t="s">
-        <v>80</v>
+      <c r="A27" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v>MainPump</v>
       </c>
       <c r="B27" s="51"/>
       <c r="C27" s="52"/>
       <c r="D27" s="53"/>
       <c r="E27" s="52"/>
       <c r="F27" s="52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.0480000000000018</v>
       </c>
       <c r="G27" s="24"/>
@@ -5719,27 +5715,28 @@
       <c r="S27" s="9"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="45" t="s">
-        <v>59</v>
+      <c r="A28" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>MP 2 Discharge</v>
       </c>
       <c r="B28" s="46">
         <f>(B11/12)*0.3048</f>
         <v>0.76200000000000001</v>
       </c>
       <c r="C28" s="54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48.768000000000001</v>
       </c>
       <c r="D28" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E28" s="54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-1.524</v>
       </c>
       <c r="F28" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5240000000000018</v>
       </c>
       <c r="H28" s="9"/>
@@ -5755,27 +5752,28 @@
       <c r="S28" s="9"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="34" t="s">
-        <v>31</v>
+      <c r="A29" s="34" t="str">
+        <f t="shared" si="2"/>
+        <v>Float Hose</v>
       </c>
       <c r="B29" s="40">
         <f>(B12/12)*0.3048</f>
         <v>0.76200000000000001</v>
       </c>
       <c r="C29" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>609.6</v>
       </c>
       <c r="D29" s="38">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="49">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="E29" s="49">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="F29" s="49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5240000000000018</v>
       </c>
       <c r="H29" s="9"/>
@@ -5791,27 +5789,28 @@
       <c r="S29" s="9"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="45" t="s">
-        <v>30</v>
+      <c r="A30" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>Riser</v>
       </c>
       <c r="B30" s="46">
         <f>(B13/12)*0.3048</f>
         <v>0.76200000000000001</v>
       </c>
       <c r="C30" s="54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39.624000000000002</v>
       </c>
       <c r="D30" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E30" s="54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-7.62</v>
       </c>
       <c r="F30" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-6.0959999999999983</v>
       </c>
       <c r="H30" s="9"/>
@@ -5827,27 +5826,28 @@
       <c r="S30" s="9"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="34" t="s">
-        <v>28</v>
+      <c r="A31" s="34" t="str">
+        <f t="shared" si="2"/>
+        <v>Subline</v>
       </c>
       <c r="B31" s="40">
         <f>(B14/12)*0.3048</f>
         <v>0.76200000000000001</v>
       </c>
       <c r="C31" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1524</v>
       </c>
       <c r="D31" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E31" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.1440000000000001</v>
       </c>
       <c r="F31" s="49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.0480000000000018</v>
       </c>
       <c r="H31" s="9"/>
@@ -5863,27 +5863,28 @@
       <c r="S31" s="9"/>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="56" t="s">
-        <v>26</v>
+      <c r="A32" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>Shore Line</v>
       </c>
       <c r="B32" s="57">
         <f>(B15/12)*0.3048</f>
         <v>0.76200000000000001</v>
       </c>
       <c r="C32" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>152.4</v>
       </c>
       <c r="D32" s="59">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="58">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="E32" s="58">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="F32" s="58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.0480000000000018</v>
       </c>
       <c r="H32" s="9"/>
@@ -5965,7 +5966,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" s="4">
         <v>60</v>
@@ -5983,7 +5984,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5" s="4">
         <v>34</v>
@@ -6001,7 +6002,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B6" s="4">
         <v>34</v>
@@ -6029,7 +6030,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B7" s="4">
         <v>300</v>
@@ -6047,10 +6048,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -6063,7 +6064,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11" s="4">
         <v>2000</v>
@@ -6116,10 +6117,10 @@
         <v>12</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J14" s="34" t="s">
         <v>23</v>
@@ -6802,12 +6803,12 @@
         <v>20</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" s="4">
         <v>84</v>
@@ -6825,7 +6826,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5" s="4">
         <v>34</v>
@@ -6843,7 +6844,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B6" s="4">
         <v>34</v>
@@ -6871,7 +6872,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B7" s="4">
         <v>315</v>
@@ -6889,10 +6890,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -6906,7 +6907,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <f>MAX(MainDriver!B4:B12)</f>
@@ -6960,10 +6961,10 @@
         <v>12</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J14" s="34" t="s">
         <v>23</v>
@@ -7637,7 +7638,7 @@
         <v>20</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -7648,7 +7649,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>23</v>
@@ -7658,7 +7659,7 @@
       <c r="A4" s="4">
         <v>200</v>
       </c>
-      <c r="B4" s="68">
+      <c r="B4" s="67">
         <v>700.00000000000011</v>
       </c>
       <c r="D4" s="38">
@@ -7674,7 +7675,7 @@
       <c r="A5" s="4">
         <v>300</v>
       </c>
-      <c r="B5" s="68">
+      <c r="B5" s="67">
         <v>950</v>
       </c>
       <c r="D5" s="38">
@@ -7690,7 +7691,7 @@
       <c r="A6" s="4">
         <v>400</v>
       </c>
-      <c r="B6" s="68">
+      <c r="B6" s="67">
         <v>1450</v>
       </c>
       <c r="D6" s="38">
@@ -7706,7 +7707,7 @@
       <c r="A7" s="4">
         <v>500</v>
       </c>
-      <c r="B7" s="68">
+      <c r="B7" s="67">
         <v>2250</v>
       </c>
       <c r="D7" s="38">
@@ -7722,7 +7723,7 @@
       <c r="A8" s="4">
         <v>600</v>
       </c>
-      <c r="B8" s="68">
+      <c r="B8" s="67">
         <v>3200</v>
       </c>
       <c r="D8" s="38">
@@ -7738,7 +7739,7 @@
       <c r="A9" s="4">
         <v>700</v>
       </c>
-      <c r="B9" s="68">
+      <c r="B9" s="67">
         <v>4400</v>
       </c>
       <c r="D9" s="38">
@@ -7754,7 +7755,7 @@
       <c r="A10" s="4">
         <v>765</v>
       </c>
-      <c r="B10" s="68">
+      <c r="B10" s="67">
         <v>4850</v>
       </c>
       <c r="D10" s="38">
@@ -7770,7 +7771,7 @@
       <c r="A11" s="4">
         <v>800</v>
       </c>
-      <c r="B11" s="68">
+      <c r="B11" s="67">
         <v>5000</v>
       </c>
       <c r="D11" s="38">
@@ -7786,7 +7787,7 @@
       <c r="A12" s="4">
         <v>900</v>
       </c>
-      <c r="B12" s="68">
+      <c r="B12" s="67">
         <v>5000</v>
       </c>
       <c r="D12" s="38">
@@ -7808,7 +7809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D933E8-A59A-4E9F-B033-19382DFDA4BB}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -7820,15 +7821,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>10</v>
@@ -7839,10 +7840,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C5" s="33">
         <v>7.4999999999999997E-2</v>
@@ -7850,10 +7851,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C6" s="33">
         <v>0.25</v>
@@ -7861,10 +7862,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>90</v>
       </c>
       <c r="C7" s="33">
         <v>0.42499999999999999</v>
@@ -7872,21 +7873,21 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="60" t="s">
         <v>94</v>
-      </c>
-      <c r="C9" s="60" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C10" s="33">
         <v>0.1</v>
@@ -7894,10 +7895,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C12" s="61">
         <v>2.65</v>
@@ -7905,10 +7906,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C13" s="61">
         <v>1.92</v>

</xml_diff>